<commit_message>
added datatable, updated data
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\Documents\DS_Projects\Analyducks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{512FCB28-063D-44E3-A026-8360F31E1ADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6307F961-DEB9-4E8C-8C24-959F784865DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EF9DEEC2-186D-4161-AB80-57C24753F6AE}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="141">
   <si>
     <t>Duck</t>
   </si>
@@ -228,9 +228,6 @@
     <t>AEPi</t>
   </si>
   <si>
-    <t>???????</t>
-  </si>
-  <si>
     <t>Bought By</t>
   </si>
   <si>
@@ -255,9 +252,6 @@
     <t>Parents</t>
   </si>
   <si>
-    <t>???</t>
-  </si>
-  <si>
     <t>Constable Quack</t>
   </si>
   <si>
@@ -438,9 +432,6 @@
     <t>Longitude</t>
   </si>
   <si>
-    <t>Fact Category</t>
-  </si>
-  <si>
     <t>Game, Set, Quack!</t>
   </si>
   <si>
@@ -462,10 +453,13 @@
     <t>Location</t>
   </si>
   <si>
-    <t>Qty</t>
-  </si>
-  <si>
     <t>Buyer</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Fun Fact</t>
   </si>
 </sst>
 </file>
@@ -544,12 +538,9 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="4">
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -580,16 +571,16 @@
     <tableColumn id="1" xr3:uid="{526AE2CE-1A5F-4A7A-B147-A0F5F581786F}" name="Duck"/>
     <tableColumn id="2" xr3:uid="{554E8660-51EE-4B26-99EE-AE8E63C39331}" name="Name"/>
     <tableColumn id="3" xr3:uid="{8490DD1D-D27A-42DB-9CD5-C2F66856608A}" name="Location"/>
-    <tableColumn id="4" xr3:uid="{3483BEC1-7940-46EA-87AB-895F2A60F5C4}" name="Date Bought" dataDxfId="4"/>
-    <tableColumn id="14" xr3:uid="{DD5702CA-A5AA-48F2-A221-5B11E7770312}" name="Latitude" dataDxfId="3"/>
-    <tableColumn id="13" xr3:uid="{6E84405B-586B-45AE-8AAB-E75DDE55DE14}" name="Longitude" dataDxfId="2"/>
-    <tableColumn id="12" xr3:uid="{DC7BB459-9BCA-4E2C-BB3A-E477F2216435}" name="Fact Category" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{D54F7BD0-C645-4075-B34E-4D059919801A}" name="Fun Fact?"/>
+    <tableColumn id="4" xr3:uid="{3483BEC1-7940-46EA-87AB-895F2A60F5C4}" name="Date Bought" dataDxfId="3"/>
+    <tableColumn id="14" xr3:uid="{DD5702CA-A5AA-48F2-A221-5B11E7770312}" name="Latitude" dataDxfId="2"/>
+    <tableColumn id="13" xr3:uid="{6E84405B-586B-45AE-8AAB-E75DDE55DE14}" name="Longitude" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{D54F7BD0-C645-4075-B34E-4D059919801A}" name="Fun Fact"/>
     <tableColumn id="6" xr3:uid="{E6929EE2-9995-48C5-99C7-C33245F8F30B}" name="Buyer"/>
-    <tableColumn id="8" xr3:uid="{291141F9-BF51-4E10-B8D7-FD40E791433E}" name="Qty"/>
+    <tableColumn id="8" xr3:uid="{291141F9-BF51-4E10-B8D7-FD40E791433E}" name="Quantity"/>
     <tableColumn id="9" xr3:uid="{B5508D8E-FAD5-4D52-8444-0DB243E6A995}" name="Weight"/>
     <tableColumn id="10" xr3:uid="{6A85F375-B028-460A-A8EB-2263E7878FF1}" name="Height"/>
     <tableColumn id="11" xr3:uid="{4F3391D1-C55C-4884-9541-D5A9A07E3C78}" name="Width"/>
+    <tableColumn id="7" xr3:uid="{71F2E7E3-9954-4C1E-AF97-3381DA18AC14}" name="Length"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -910,10 +901,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B28BE0B7-C424-43DE-B13E-D21D7F7285C7}">
-  <dimension ref="A1:O40"/>
+  <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -922,62 +913,61 @@
     <col min="2" max="2" width="35.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="34.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5546875" customWidth="1"/>
-    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" customWidth="1"/>
+    <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
+      </c>
+      <c r="G1" t="s">
+        <v>140</v>
       </c>
       <c r="H1" t="s">
-        <v>39</v>
+        <v>138</v>
       </c>
       <c r="I1" t="s">
-        <v>142</v>
+        <v>74</v>
       </c>
       <c r="J1" t="s">
-        <v>141</v>
+        <v>104</v>
       </c>
       <c r="K1" t="s">
-        <v>106</v>
+        <v>125</v>
       </c>
       <c r="L1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="M1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>128</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>130</v>
       </c>
       <c r="C2" t="s">
         <v>41</v>
@@ -992,34 +982,34 @@
         <v>-77.025510999999995</v>
       </c>
       <c r="G2" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="H2" t="s">
-        <v>48</v>
-      </c>
-      <c r="I2" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="K2">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="L2">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="M2">
-        <v>2</v>
-      </c>
-      <c r="O2" s="2"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+      <c r="N2" s="2"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C3" t="s">
         <v>42</v>
@@ -1034,34 +1024,34 @@
         <v>2.340983</v>
       </c>
       <c r="G3" t="s">
-        <v>72</v>
+        <v>116</v>
       </c>
       <c r="H3" t="s">
-        <v>118</v>
-      </c>
-      <c r="I3" t="s">
-        <v>67</v>
+        <v>66</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="K3">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="L3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="M3">
-        <v>5</v>
-      </c>
-      <c r="O3" s="2"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="N3" s="2"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C4" t="s">
         <v>43</v>
@@ -1076,33 +1066,33 @@
         <v>34.775413</v>
       </c>
       <c r="G4" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="H4" t="s">
-        <v>48</v>
-      </c>
-      <c r="I4" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="K4">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="L4">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="M4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C5" t="s">
         <v>44</v>
@@ -1117,34 +1107,34 @@
         <v>-73.846541999999999</v>
       </c>
       <c r="G5" t="s">
-        <v>72</v>
+        <v>131</v>
       </c>
       <c r="H5" t="s">
-        <v>134</v>
-      </c>
-      <c r="I5" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
       </c>
       <c r="J5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K5">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="L5">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="M5">
-        <v>7</v>
-      </c>
-      <c r="O5" s="2"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+      <c r="N5" s="2"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C6" t="s">
         <v>45</v>
@@ -1159,37 +1149,37 @@
         <v>-72.624831999999998</v>
       </c>
       <c r="G6" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="H6" t="s">
-        <v>48</v>
-      </c>
-      <c r="I6" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+      <c r="I6">
+        <v>2</v>
       </c>
       <c r="J6">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="K6">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="L6">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="M6">
         <v>5</v>
       </c>
-      <c r="O6" s="2"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N6" s="2"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D7" s="1">
         <v>43160</v>
@@ -1201,28 +1191,28 @@
         <v>-77.089934999999997</v>
       </c>
       <c r="G7" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="H7" t="s">
-        <v>48</v>
-      </c>
-      <c r="I7" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+      <c r="I7">
+        <v>12</v>
       </c>
       <c r="J7">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="K7">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="L7">
+        <v>8</v>
+      </c>
+      <c r="M7">
         <v>2</v>
       </c>
-      <c r="M7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1242,40 +1232,40 @@
         <v>-71.147199000000001</v>
       </c>
       <c r="G8" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="H8" t="s">
-        <v>48</v>
-      </c>
-      <c r="I8" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
       </c>
       <c r="J8">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="K8">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="L8">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="M8">
-        <v>2</v>
-      </c>
-      <c r="O8" s="2"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="N8" s="2"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C9" t="s">
         <v>46</v>
       </c>
       <c r="D9" s="1">
-        <v>47484</v>
+        <v>44713</v>
       </c>
       <c r="E9" s="5">
         <v>42.395432</v>
@@ -1284,34 +1274,34 @@
         <v>-71.147199000000001</v>
       </c>
       <c r="G9" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="H9" t="s">
-        <v>48</v>
-      </c>
-      <c r="I9" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
       </c>
       <c r="J9">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K9">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="L9">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="M9">
-        <v>2</v>
-      </c>
-      <c r="O9" s="2"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+      <c r="N9" s="2"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C10" t="s">
         <v>49</v>
@@ -1326,39 +1316,39 @@
         <v>-90.489697000000007</v>
       </c>
       <c r="G10" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="H10" t="s">
-        <v>48</v>
-      </c>
-      <c r="I10" t="s">
-        <v>68</v>
+        <v>67</v>
+      </c>
+      <c r="I10">
+        <v>6</v>
       </c>
       <c r="J10">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="K10">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="L10">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="M10">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C11" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D11" s="1">
-        <v>47484</v>
+        <v>44828</v>
       </c>
       <c r="E11" s="4">
         <v>42.864286999999997</v>
@@ -1367,34 +1357,34 @@
         <v>-71.625247999999999</v>
       </c>
       <c r="G11" t="s">
-        <v>72</v>
+        <v>100</v>
       </c>
       <c r="H11" t="s">
-        <v>102</v>
-      </c>
-      <c r="I11" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
       </c>
       <c r="J11">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="K11">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="L11">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="M11">
-        <v>1</v>
-      </c>
-      <c r="O11" s="2"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="N11" s="2"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B12" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C12" t="s">
         <v>50</v>
@@ -1409,29 +1399,29 @@
         <v>-71.208479999999994</v>
       </c>
       <c r="G12" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="H12" t="s">
-        <v>48</v>
-      </c>
-      <c r="I12" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
       </c>
       <c r="J12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K12">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="L12">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="M12">
-        <v>2</v>
-      </c>
-      <c r="O12" s="2"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+      <c r="N12" s="2"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1451,33 +1441,33 @@
         <v>-70.667964999999995</v>
       </c>
       <c r="G13" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="H13" t="s">
-        <v>48</v>
-      </c>
-      <c r="I13" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
       </c>
       <c r="J13">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="K13">
         <v>6</v>
       </c>
       <c r="L13">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="M13">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C14" t="s">
         <v>52</v>
@@ -1492,34 +1482,34 @@
         <v>-73.996746999999999</v>
       </c>
       <c r="G14" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="H14" t="s">
-        <v>48</v>
-      </c>
-      <c r="I14" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
       </c>
       <c r="J14">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K14">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="L14">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="M14">
         <v>1</v>
       </c>
-      <c r="O14" s="2"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N14" s="2"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C15" t="s">
         <v>53</v>
@@ -1534,34 +1524,34 @@
         <v>-74.044548000000006</v>
       </c>
       <c r="G15" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="H15" t="s">
-        <v>48</v>
-      </c>
-      <c r="I15" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
       </c>
       <c r="J15">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="K15">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="L15">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="M15">
-        <v>4</v>
-      </c>
-      <c r="O15" s="2"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="N15" s="2"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C16" t="s">
         <v>54</v>
@@ -1576,33 +1566,33 @@
         <v>-0.12764700000000001</v>
       </c>
       <c r="G16" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="H16" t="s">
-        <v>48</v>
-      </c>
-      <c r="I16" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
       </c>
       <c r="J16">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="K16">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L16">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="M16">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C17" t="s">
         <v>43</v>
@@ -1617,34 +1607,34 @@
         <v>34.775413</v>
       </c>
       <c r="G17" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="H17" t="s">
-        <v>48</v>
-      </c>
-      <c r="I17" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
       </c>
       <c r="J17">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="K17">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="L17">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="M17">
-        <v>6</v>
-      </c>
-      <c r="O17" s="2"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+      <c r="N17" s="2"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C18" t="s">
         <v>55</v>
@@ -1659,34 +1649,34 @@
         <v>-70.854718000000005</v>
       </c>
       <c r="G18" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="H18" t="s">
-        <v>48</v>
-      </c>
-      <c r="I18" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
       </c>
       <c r="J18">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="K18">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="L18">
+        <v>8</v>
+      </c>
+      <c r="M18">
         <v>4</v>
       </c>
-      <c r="M18">
-        <v>7</v>
-      </c>
-      <c r="O18" s="2"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N18" s="2"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C19" t="s">
         <v>56</v>
@@ -1701,33 +1691,33 @@
         <v>2.1743480000000002</v>
       </c>
       <c r="G19" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="H19" t="s">
-        <v>48</v>
-      </c>
-      <c r="I19" t="s">
-        <v>69</v>
+        <v>68</v>
+      </c>
+      <c r="I19">
+        <v>2</v>
       </c>
       <c r="J19">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="K19">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="L19">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="M19">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C20" t="s">
         <v>46</v>
@@ -1742,34 +1732,34 @@
         <v>-71.147199000000001</v>
       </c>
       <c r="G20" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="H20" t="s">
-        <v>78</v>
-      </c>
-      <c r="I20" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
       </c>
       <c r="J20">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="K20">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="L20">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="M20">
-        <v>6</v>
-      </c>
-      <c r="O20" s="2"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="N20" s="2"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C21" t="s">
         <v>43</v>
@@ -1784,75 +1774,75 @@
         <v>34.775413</v>
       </c>
       <c r="G21" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="H21" t="s">
-        <v>48</v>
-      </c>
-      <c r="I21" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
       </c>
       <c r="J21">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="K21">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="L21">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="M21">
-        <v>5</v>
-      </c>
-      <c r="O21" s="2"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="N21" s="2"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C22" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="D22" s="1">
-        <v>44682</v>
+        <v>44787</v>
       </c>
       <c r="E22" s="4">
-        <v>32.074058999999998</v>
+        <v>45.505358000000001</v>
       </c>
       <c r="F22" s="3">
-        <v>34.775413</v>
+        <v>-73.554688999999996</v>
       </c>
       <c r="G22" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="H22" t="s">
-        <v>48</v>
-      </c>
-      <c r="I22" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
       </c>
       <c r="J22">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="K22">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="L22">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="M22">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>37</v>
       </c>
       <c r="B23" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C23" t="s">
         <v>41</v>
@@ -1867,34 +1857,34 @@
         <v>-77.025510999999995</v>
       </c>
       <c r="G23" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="H23" t="s">
-        <v>91</v>
-      </c>
-      <c r="I23" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
       </c>
       <c r="J23">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="K23">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="L23">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="M23">
-        <v>4</v>
-      </c>
-      <c r="O23" s="2"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+      <c r="N23" s="2"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C24" t="s">
         <v>57</v>
@@ -1909,40 +1899,40 @@
         <v>-80.526619999999994</v>
       </c>
       <c r="G24" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="H24" t="s">
-        <v>88</v>
-      </c>
-      <c r="I24" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
       </c>
       <c r="J24">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="K24">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="L24">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M24">
-        <v>6</v>
-      </c>
-      <c r="O24" s="2"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="N24" s="2"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C25" t="s">
         <v>58</v>
       </c>
       <c r="D25" s="1">
-        <v>44774</v>
+        <v>44787</v>
       </c>
       <c r="E25" s="4">
         <v>45.505358000000001</v>
@@ -1951,33 +1941,33 @@
         <v>-73.554688999999996</v>
       </c>
       <c r="G25" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="H25" t="s">
-        <v>90</v>
-      </c>
-      <c r="I25" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="I25">
+        <v>1</v>
       </c>
       <c r="J25">
         <v>1</v>
       </c>
       <c r="K25">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="L25">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="M25">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C26" t="s">
         <v>46</v>
@@ -1992,34 +1982,34 @@
         <v>-71.147199000000001</v>
       </c>
       <c r="G26" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="H26" t="s">
-        <v>48</v>
-      </c>
-      <c r="I26" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
       </c>
       <c r="J26">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="K26">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="L26">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="M26">
-        <v>2</v>
-      </c>
-      <c r="O26" s="2"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+      <c r="N26" s="2"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>24</v>
       </c>
       <c r="B27" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C27" t="s">
         <v>59</v>
@@ -2034,37 +2024,37 @@
         <v>-77.111007000000001</v>
       </c>
       <c r="G27" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="H27" t="s">
-        <v>48</v>
-      </c>
-      <c r="I27" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
       </c>
       <c r="J27">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="K27">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="L27">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="M27">
-        <v>7</v>
-      </c>
-      <c r="O27" s="2"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="N27" s="2"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B28" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C28" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D28" s="1">
         <v>43617</v>
@@ -2076,28 +2066,28 @@
         <v>16.372503999999999</v>
       </c>
       <c r="G28" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="H28" t="s">
-        <v>48</v>
-      </c>
-      <c r="I28" t="s">
-        <v>71</v>
+        <v>70</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
       </c>
       <c r="J28">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="K28">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="L28">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="M28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -2117,37 +2107,37 @@
         <v>-77.039688999999996</v>
       </c>
       <c r="G29" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="H29" t="s">
-        <v>48</v>
-      </c>
-      <c r="I29" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
       </c>
       <c r="J29">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="K29">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="L29">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M29">
-        <v>2</v>
-      </c>
-      <c r="O29" s="2"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="N29" s="2"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C30" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D30" s="1">
         <v>44682</v>
@@ -2159,34 +2149,34 @@
         <v>35.203386999999999</v>
       </c>
       <c r="G30" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="H30" t="s">
-        <v>48</v>
-      </c>
-      <c r="I30" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+      <c r="I30">
+        <v>1</v>
       </c>
       <c r="J30">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="K30">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="L30">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="M30">
-        <v>5</v>
-      </c>
-      <c r="O30" s="2"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+      <c r="N30" s="2"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C31" t="s">
         <v>43</v>
@@ -2201,33 +2191,33 @@
         <v>34.775413</v>
       </c>
       <c r="G31" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="H31" t="s">
-        <v>48</v>
-      </c>
-      <c r="I31" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+      <c r="I31">
+        <v>1</v>
       </c>
       <c r="J31">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="K31">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="L31">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="M31">
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>29</v>
       </c>
       <c r="B32" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C32" t="s">
         <v>46</v>
@@ -2242,34 +2232,34 @@
         <v>-71.147199000000001</v>
       </c>
       <c r="G32" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="H32" t="s">
-        <v>48</v>
-      </c>
-      <c r="I32" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+      <c r="I32">
+        <v>1</v>
       </c>
       <c r="J32">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K32">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="L32">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="M32">
-        <v>5</v>
-      </c>
-      <c r="O32" s="2"/>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+      <c r="N32" s="2"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>30</v>
       </c>
       <c r="B33" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C33" t="s">
         <v>61</v>
@@ -2284,34 +2274,34 @@
         <v>-70.892773000000005</v>
       </c>
       <c r="G33" t="s">
-        <v>72</v>
+        <v>127</v>
       </c>
       <c r="H33" t="s">
-        <v>129</v>
-      </c>
-      <c r="I33" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+      <c r="I33">
+        <v>1</v>
       </c>
       <c r="J33">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="K33">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="L33">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="M33">
-        <v>6</v>
-      </c>
-      <c r="O33" s="2"/>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+      <c r="N33" s="2"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C34" t="s">
         <v>62</v>
@@ -2326,33 +2316,33 @@
         <v>-79.942740999999998</v>
       </c>
       <c r="G34" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="H34" t="s">
-        <v>48</v>
-      </c>
-      <c r="I34" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+      <c r="I34">
+        <v>1</v>
       </c>
       <c r="J34">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="K34">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L34">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="M34">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C35" t="s">
         <v>41</v>
@@ -2367,37 +2357,37 @@
         <v>-77.025510999999995</v>
       </c>
       <c r="G35" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="H35" t="s">
-        <v>48</v>
-      </c>
-      <c r="I35" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+      <c r="I35">
+        <v>1</v>
       </c>
       <c r="J35">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="K35">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="L35">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="M35">
-        <v>7</v>
-      </c>
-      <c r="O35" s="2"/>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="N35" s="2"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>33</v>
       </c>
       <c r="B36" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C36" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D36" s="1">
         <v>44803</v>
@@ -2409,29 +2399,29 @@
         <v>-70.895891000000006</v>
       </c>
       <c r="G36" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="H36" t="s">
-        <v>48</v>
-      </c>
-      <c r="I36" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+      <c r="I36">
+        <v>1</v>
       </c>
       <c r="J36">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="K36">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="L36">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="M36">
         <v>2</v>
       </c>
-      <c r="O36" s="2"/>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N36" s="2"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>34</v>
       </c>
@@ -2439,76 +2429,84 @@
         <v>48</v>
       </c>
       <c r="C37" t="s">
-        <v>63</v>
+        <v>133</v>
       </c>
       <c r="D37" s="1">
-        <v>47484</v>
-      </c>
-      <c r="E37" s="4"/>
-      <c r="F37" s="3"/>
+        <v>44762</v>
+      </c>
+      <c r="E37" s="4">
+        <v>42.522075000000001</v>
+      </c>
+      <c r="F37" s="3">
+        <v>-70.895891000000006</v>
+      </c>
       <c r="G37" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="H37" t="s">
-        <v>48</v>
-      </c>
-      <c r="I37" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+      <c r="I37">
+        <v>1</v>
       </c>
       <c r="J37">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="K37">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="L37">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="M37">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C38" t="s">
-        <v>63</v>
+        <v>132</v>
       </c>
       <c r="D38" s="1">
-        <v>47484</v>
-      </c>
-      <c r="E38" s="4"/>
-      <c r="F38" s="3"/>
+        <v>44829</v>
+      </c>
+      <c r="E38" s="4">
+        <v>42.864286999999997</v>
+      </c>
+      <c r="F38" s="3">
+        <v>-71.625247999999999</v>
+      </c>
       <c r="G38" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="H38" t="s">
-        <v>48</v>
-      </c>
-      <c r="I38" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="I38">
+        <v>1</v>
       </c>
       <c r="J38">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="K38">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="L38">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="M38">
-        <v>3</v>
-      </c>
-      <c r="O38" s="2"/>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="N38" s="2"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B39" t="s">
         <v>48</v>
@@ -2526,31 +2524,31 @@
         <v>-71.191412</v>
       </c>
       <c r="G39" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="H39" t="s">
-        <v>48</v>
-      </c>
-      <c r="I39" t="s">
-        <v>126</v>
+        <v>124</v>
+      </c>
+      <c r="I39">
+        <v>1</v>
       </c>
       <c r="J39">
         <v>1</v>
       </c>
       <c r="K39">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="L39">
         <v>3</v>
       </c>
       <c r="M39">
-        <v>4</v>
-      </c>
-      <c r="O39" s="2"/>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="N39" s="2"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B40" t="s">
         <v>48</v>
@@ -2568,25 +2566,25 @@
         <v>-71.191412</v>
       </c>
       <c r="G40" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="H40" t="s">
-        <v>48</v>
-      </c>
-      <c r="I40" t="s">
-        <v>126</v>
+        <v>124</v>
+      </c>
+      <c r="I40">
+        <v>1</v>
       </c>
       <c r="J40">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="K40">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="L40">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="M40">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -2622,10 +2620,10 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C1" t="s">
         <v>38</v>
@@ -2637,21 +2635,21 @@
         <v>39</v>
       </c>
       <c r="F1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" t="s">
         <v>64</v>
       </c>
-      <c r="G1" t="s">
-        <v>65</v>
-      </c>
       <c r="H1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D2" s="1"/>
     </row>
@@ -2666,7 +2664,7 @@
         <v>44835</v>
       </c>
       <c r="F3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -2683,7 +2681,7 @@
         <v>44835</v>
       </c>
       <c r="F4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -2691,43 +2689,43 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D11" s="1"/>
     </row>

</xml_diff>

<commit_message>
added chart and axis titles
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\Documents\DS_Projects\Analyducks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6307F961-DEB9-4E8C-8C24-959F784865DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA65B57-6719-4D33-A62C-59433A580CF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EF9DEEC2-186D-4161-AB80-57C24753F6AE}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="143">
   <si>
     <t>Duck</t>
   </si>
@@ -460,6 +460,12 @@
   </si>
   <si>
     <t>Fun Fact</t>
+  </si>
+  <si>
+    <t>Total_Weight</t>
+  </si>
+  <si>
+    <t>Date_Bought</t>
   </si>
 </sst>
 </file>
@@ -571,13 +577,13 @@
     <tableColumn id="1" xr3:uid="{526AE2CE-1A5F-4A7A-B147-A0F5F581786F}" name="Duck"/>
     <tableColumn id="2" xr3:uid="{554E8660-51EE-4B26-99EE-AE8E63C39331}" name="Name"/>
     <tableColumn id="3" xr3:uid="{8490DD1D-D27A-42DB-9CD5-C2F66856608A}" name="Location"/>
-    <tableColumn id="4" xr3:uid="{3483BEC1-7940-46EA-87AB-895F2A60F5C4}" name="Date Bought" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{3483BEC1-7940-46EA-87AB-895F2A60F5C4}" name="Date_Bought" dataDxfId="3"/>
     <tableColumn id="14" xr3:uid="{DD5702CA-A5AA-48F2-A221-5B11E7770312}" name="Latitude" dataDxfId="2"/>
     <tableColumn id="13" xr3:uid="{6E84405B-586B-45AE-8AAB-E75DDE55DE14}" name="Longitude" dataDxfId="1"/>
     <tableColumn id="5" xr3:uid="{D54F7BD0-C645-4075-B34E-4D059919801A}" name="Fun Fact"/>
     <tableColumn id="6" xr3:uid="{E6929EE2-9995-48C5-99C7-C33245F8F30B}" name="Buyer"/>
     <tableColumn id="8" xr3:uid="{291141F9-BF51-4E10-B8D7-FD40E791433E}" name="Quantity"/>
-    <tableColumn id="9" xr3:uid="{B5508D8E-FAD5-4D52-8444-0DB243E6A995}" name="Weight"/>
+    <tableColumn id="9" xr3:uid="{B5508D8E-FAD5-4D52-8444-0DB243E6A995}" name="Total_Weight"/>
     <tableColumn id="10" xr3:uid="{6A85F375-B028-460A-A8EB-2263E7878FF1}" name="Height"/>
     <tableColumn id="11" xr3:uid="{4F3391D1-C55C-4884-9541-D5A9A07E3C78}" name="Width"/>
     <tableColumn id="7" xr3:uid="{71F2E7E3-9954-4C1E-AF97-3381DA18AC14}" name="Length"/>
@@ -904,7 +910,7 @@
   <dimension ref="A1:N40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -932,7 +938,7 @@
         <v>137</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>40</v>
+        <v>142</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>129</v>
@@ -950,7 +956,7 @@
         <v>74</v>
       </c>
       <c r="J1" t="s">
-        <v>104</v>
+        <v>141</v>
       </c>
       <c r="K1" t="s">
         <v>125</v>

</xml_diff>

<commit_message>
added two more kpi cards, and styling
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\Documents\DS_Projects\Analyducks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA65B57-6719-4D33-A62C-59433A580CF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABD4895B-D61C-48F2-8F79-D0057E433F48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EF9DEEC2-186D-4161-AB80-57C24753F6AE}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="182">
   <si>
     <t>Duck</t>
   </si>
@@ -162,21 +162,12 @@
     <t>Date Bought</t>
   </si>
   <si>
-    <t>Spy Museum</t>
-  </si>
-  <si>
     <t>Paris</t>
   </si>
   <si>
     <t>Israel</t>
   </si>
   <si>
-    <t>NY US Open</t>
-  </si>
-  <si>
-    <t>Big E</t>
-  </si>
-  <si>
     <t>Fuse</t>
   </si>
   <si>
@@ -186,45 +177,12 @@
     <t>????????</t>
   </si>
   <si>
-    <t>STL</t>
-  </si>
-  <si>
-    <t>Burlington</t>
-  </si>
-  <si>
-    <t>Plymouth musem</t>
-  </si>
-  <si>
-    <t>Cruise Ship</t>
-  </si>
-  <si>
-    <t>NY Trip</t>
-  </si>
-  <si>
-    <t>London</t>
-  </si>
-  <si>
-    <t>ice cream marblehead</t>
-  </si>
-  <si>
     <t>Spain</t>
   </si>
   <si>
-    <t>Cape Canaveral</t>
-  </si>
-  <si>
     <t>Montreal</t>
   </si>
   <si>
-    <t>Ballston</t>
-  </si>
-  <si>
-    <t>DCA</t>
-  </si>
-  <si>
-    <t>NY Essex Pizza Salem</t>
-  </si>
-  <si>
     <t>AEPi</t>
   </si>
   <si>
@@ -384,9 +342,6 @@
     <t>Cannes-ard</t>
   </si>
   <si>
-    <t>Duck Lord / Lord of the wings</t>
-  </si>
-  <si>
     <t>je ne sais quack</t>
   </si>
   <si>
@@ -438,21 +393,9 @@
     <t>Amherst, NH</t>
   </si>
   <si>
-    <t>Koto Salem</t>
-  </si>
-  <si>
-    <t>Bethesda</t>
-  </si>
-  <si>
-    <t>Israel museum, Jerusalem</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Location</t>
-  </si>
-  <si>
     <t>Buyer</t>
   </si>
   <si>
@@ -466,6 +409,180 @@
   </si>
   <si>
     <t>Date_Bought</t>
+  </si>
+  <si>
+    <t>International Spy Museum</t>
+  </si>
+  <si>
+    <t>Bethesda, MD</t>
+  </si>
+  <si>
+    <t>St. Louis, MO</t>
+  </si>
+  <si>
+    <t>Purchase_Method</t>
+  </si>
+  <si>
+    <t>Purchase_Retailer</t>
+  </si>
+  <si>
+    <t>Phyiscal Store</t>
+  </si>
+  <si>
+    <t>Online</t>
+  </si>
+  <si>
+    <t>Duck You</t>
+  </si>
+  <si>
+    <t>Paris Duck Store</t>
+  </si>
+  <si>
+    <t>US Open</t>
+  </si>
+  <si>
+    <t>Food Truck</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>Lego Store</t>
+  </si>
+  <si>
+    <t>Plymouth Patuxet Museum</t>
+  </si>
+  <si>
+    <t>Gift Shop</t>
+  </si>
+  <si>
+    <t>Norwegian Cruise Line</t>
+  </si>
+  <si>
+    <t>Barcelona Duck Store</t>
+  </si>
+  <si>
+    <t>JustGeek</t>
+  </si>
+  <si>
+    <t>Le Letit Duck Shoppe</t>
+  </si>
+  <si>
+    <t>NASA Cape Canaveral</t>
+  </si>
+  <si>
+    <t>Etsy</t>
+  </si>
+  <si>
+    <t>CVS</t>
+  </si>
+  <si>
+    <t>Vienna Gift Shop</t>
+  </si>
+  <si>
+    <t>DCA Airport</t>
+  </si>
+  <si>
+    <t>The Israel Museum</t>
+  </si>
+  <si>
+    <t>Claw Machine</t>
+  </si>
+  <si>
+    <t>Reserve at Burlington</t>
+  </si>
+  <si>
+    <t>Burlington, MA</t>
+  </si>
+  <si>
+    <t>Salem, MA</t>
+  </si>
+  <si>
+    <t>Washington, DC</t>
+  </si>
+  <si>
+    <t>West Springfield, MA</t>
+  </si>
+  <si>
+    <t>Cambridge, MA</t>
+  </si>
+  <si>
+    <t>Plymouth, MA</t>
+  </si>
+  <si>
+    <t>New York City, NY</t>
+  </si>
+  <si>
+    <t>Marblehead, MA</t>
+  </si>
+  <si>
+    <t>Cape Canaveral, FL</t>
+  </si>
+  <si>
+    <t>Ballston, VA</t>
+  </si>
+  <si>
+    <t>Billgrim</t>
+  </si>
+  <si>
+    <t>Classic Quack</t>
+  </si>
+  <si>
+    <t>UniQuack</t>
+  </si>
+  <si>
+    <t>Lord of the Wings</t>
+  </si>
+  <si>
+    <t>Unknown Store</t>
+  </si>
+  <si>
+    <t>Gas Station</t>
+  </si>
+  <si>
+    <t>Terry's Old Fashion Ice Cream Shop</t>
+  </si>
+  <si>
+    <t>New York Essex Pizza</t>
+  </si>
+  <si>
+    <t>Duck Game</t>
+  </si>
+  <si>
+    <t>Koto Grill &amp; Sushi</t>
+  </si>
+  <si>
+    <t>Purchase_Country</t>
+  </si>
+  <si>
+    <t>Purchase_City</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Tel Aviv</t>
+  </si>
+  <si>
+    <t>Pittsburgh, PA</t>
+  </si>
+  <si>
+    <t>Londong</t>
+  </si>
+  <si>
+    <t>England</t>
+  </si>
+  <si>
+    <t>Barcelona</t>
+  </si>
+  <si>
+    <t>Vienna</t>
+  </si>
+  <si>
+    <t>Jerusalem</t>
   </si>
 </sst>
 </file>
@@ -571,12 +688,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{55715085-9AFB-4516-817F-DC3F49C2B133}" name="Table1" displayName="Table1" ref="A1:M40" totalsRowShown="0">
-  <autoFilter ref="A1:M40" xr:uid="{55715085-9AFB-4516-817F-DC3F49C2B133}"/>
-  <tableColumns count="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{55715085-9AFB-4516-817F-DC3F49C2B133}" name="Table1" displayName="Table1" ref="A1:P40" totalsRowShown="0">
+  <autoFilter ref="A1:P40" xr:uid="{55715085-9AFB-4516-817F-DC3F49C2B133}"/>
+  <tableColumns count="16">
     <tableColumn id="1" xr3:uid="{526AE2CE-1A5F-4A7A-B147-A0F5F581786F}" name="Duck"/>
     <tableColumn id="2" xr3:uid="{554E8660-51EE-4B26-99EE-AE8E63C39331}" name="Name"/>
-    <tableColumn id="3" xr3:uid="{8490DD1D-D27A-42DB-9CD5-C2F66856608A}" name="Location"/>
+    <tableColumn id="12" xr3:uid="{1C472003-62CC-42E3-90B6-7C966E890961}" name="Purchase_Method"/>
+    <tableColumn id="15" xr3:uid="{4B3C55F4-1E57-46AC-A19E-4EBB1DF50BEC}" name="Purchase_Retailer"/>
+    <tableColumn id="3" xr3:uid="{8490DD1D-D27A-42DB-9CD5-C2F66856608A}" name="Purchase_City"/>
+    <tableColumn id="16" xr3:uid="{8F6D77DD-9950-4A0C-9650-EF78F2440AF5}" name="Purchase_Country"/>
     <tableColumn id="4" xr3:uid="{3483BEC1-7940-46EA-87AB-895F2A60F5C4}" name="Date_Bought" dataDxfId="3"/>
     <tableColumn id="14" xr3:uid="{DD5702CA-A5AA-48F2-A221-5B11E7770312}" name="Latitude" dataDxfId="2"/>
     <tableColumn id="13" xr3:uid="{6E84405B-586B-45AE-8AAB-E75DDE55DE14}" name="Longitude" dataDxfId="1"/>
@@ -907,1689 +1027,2049 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B28BE0B7-C424-43DE-B13E-D21D7F7285C7}">
-  <dimension ref="A1:N40"/>
+  <dimension ref="A1:Q40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="B23" zoomScale="114" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="34.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.5546875" customWidth="1"/>
-    <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="35.44140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="E1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="J1" t="s">
+        <v>121</v>
+      </c>
+      <c r="K1" t="s">
+        <v>119</v>
+      </c>
+      <c r="L1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O1" t="s">
+        <v>111</v>
+      </c>
+      <c r="P1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" t="s">
         <v>129</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="G1" t="s">
-        <v>140</v>
-      </c>
-      <c r="H1" t="s">
-        <v>138</v>
-      </c>
-      <c r="I1" t="s">
-        <v>74</v>
-      </c>
-      <c r="J1" t="s">
-        <v>141</v>
-      </c>
-      <c r="K1" t="s">
-        <v>125</v>
-      </c>
-      <c r="L1" t="s">
-        <v>126</v>
-      </c>
-      <c r="M1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>128</v>
-      </c>
-      <c r="C2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" s="1">
+      <c r="D2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E2" t="s">
+        <v>153</v>
+      </c>
+      <c r="F2" t="s">
+        <v>173</v>
+      </c>
+      <c r="G2" s="1">
         <v>43134</v>
       </c>
-      <c r="E2" s="4">
+      <c r="H2" s="4">
         <v>38.883940000000003</v>
       </c>
-      <c r="F2" s="3">
+      <c r="I2" s="3">
         <v>-77.025510999999995</v>
       </c>
-      <c r="G2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H2" t="s">
-        <v>65</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
+      <c r="J2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K2" t="s">
+        <v>51</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
         <v>7</v>
       </c>
-      <c r="K2">
+      <c r="N2">
         <v>14</v>
       </c>
-      <c r="L2">
+      <c r="O2">
         <v>24</v>
       </c>
-      <c r="M2">
+      <c r="P2">
         <v>21</v>
       </c>
-      <c r="N2" s="2"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="Q2" s="2"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D3" s="1">
+        <v>129</v>
+      </c>
+      <c r="D3" t="s">
+        <v>132</v>
+      </c>
+      <c r="E3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" t="s">
+        <v>174</v>
+      </c>
+      <c r="G3" s="1">
         <v>44743</v>
       </c>
-      <c r="E3" s="4">
+      <c r="H3" s="4">
         <v>48.884098000000002</v>
       </c>
-      <c r="F3" s="3">
+      <c r="I3" s="3">
         <v>2.340983</v>
       </c>
-      <c r="G3" t="s">
-        <v>116</v>
-      </c>
-      <c r="H3" t="s">
-        <v>66</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
+      <c r="J3" t="s">
+        <v>101</v>
+      </c>
+      <c r="K3" t="s">
+        <v>52</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
         <v>10</v>
       </c>
-      <c r="K3">
+      <c r="N3">
         <v>22</v>
       </c>
-      <c r="L3">
+      <c r="O3">
         <v>2</v>
       </c>
-      <c r="M3">
+      <c r="P3">
         <v>12</v>
       </c>
-      <c r="N3" s="2"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="Q3" s="2"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D4" s="1">
+        <v>129</v>
+      </c>
+      <c r="D4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E4" t="s">
+        <v>175</v>
+      </c>
+      <c r="F4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="1">
         <v>44682</v>
       </c>
-      <c r="E4" s="4">
+      <c r="H4" s="4">
         <v>32.074058999999998</v>
       </c>
-      <c r="F4" s="3">
+      <c r="I4" s="3">
         <v>34.775413</v>
       </c>
-      <c r="G4" t="s">
-        <v>48</v>
-      </c>
-      <c r="H4" t="s">
-        <v>65</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4">
+      <c r="J4" t="s">
+        <v>45</v>
+      </c>
+      <c r="K4" t="s">
+        <v>51</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
         <v>20</v>
       </c>
-      <c r="K4">
+      <c r="N4">
         <v>15</v>
       </c>
-      <c r="L4">
+      <c r="O4">
         <v>14</v>
       </c>
-      <c r="M4">
+      <c r="P4">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" s="1">
+        <v>129</v>
+      </c>
+      <c r="D5" t="s">
+        <v>133</v>
+      </c>
+      <c r="E5" t="s">
+        <v>157</v>
+      </c>
+      <c r="F5" t="s">
+        <v>173</v>
+      </c>
+      <c r="G5" s="1">
         <v>42979</v>
       </c>
-      <c r="E5" s="5">
+      <c r="H5" s="5">
         <v>40.749575999999998</v>
       </c>
-      <c r="F5" s="3">
+      <c r="I5" s="3">
         <v>-73.846541999999999</v>
       </c>
-      <c r="G5" t="s">
-        <v>131</v>
-      </c>
-      <c r="H5" t="s">
-        <v>65</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="J5">
+      <c r="J5" t="s">
+        <v>116</v>
+      </c>
+      <c r="K5" t="s">
+        <v>51</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
         <v>4</v>
       </c>
-      <c r="K5">
+      <c r="N5">
         <v>14</v>
       </c>
-      <c r="L5">
+      <c r="O5">
         <v>18</v>
       </c>
-      <c r="M5">
+      <c r="P5">
         <v>17</v>
       </c>
-      <c r="N5" s="2"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="Q5" s="2"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" s="1">
+        <v>129</v>
+      </c>
+      <c r="D6" t="s">
+        <v>134</v>
+      </c>
+      <c r="E6" t="s">
+        <v>154</v>
+      </c>
+      <c r="F6" t="s">
+        <v>173</v>
+      </c>
+      <c r="G6" s="1">
         <v>44805</v>
       </c>
-      <c r="E6" s="5">
+      <c r="H6" s="5">
         <v>42.091304999999998</v>
       </c>
-      <c r="F6" s="3">
+      <c r="I6" s="3">
         <v>-72.624831999999998</v>
       </c>
-      <c r="G6" t="s">
-        <v>48</v>
-      </c>
-      <c r="H6" t="s">
-        <v>65</v>
-      </c>
-      <c r="I6">
+      <c r="J6" t="s">
+        <v>45</v>
+      </c>
+      <c r="K6" t="s">
+        <v>51</v>
+      </c>
+      <c r="L6">
         <v>2</v>
       </c>
-      <c r="J6">
+      <c r="M6">
         <v>22</v>
       </c>
-      <c r="K6">
+      <c r="N6">
         <v>21</v>
       </c>
-      <c r="L6">
+      <c r="O6">
         <v>9</v>
       </c>
-      <c r="M6">
+      <c r="P6">
         <v>5</v>
       </c>
-      <c r="N6" s="2"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="Q6" s="2"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="C7" t="s">
-        <v>134</v>
-      </c>
-      <c r="D7" s="1">
+        <v>130</v>
+      </c>
+      <c r="D7" t="s">
+        <v>135</v>
+      </c>
+      <c r="E7" t="s">
+        <v>125</v>
+      </c>
+      <c r="F7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G7" s="1">
         <v>43160</v>
       </c>
-      <c r="E7" s="4">
+      <c r="H7" s="4">
         <v>38.984665999999997</v>
       </c>
-      <c r="F7" s="3">
+      <c r="I7" s="3">
         <v>-77.089934999999997</v>
       </c>
-      <c r="G7" t="s">
-        <v>48</v>
-      </c>
-      <c r="H7" t="s">
-        <v>65</v>
-      </c>
-      <c r="I7">
+      <c r="J7" t="s">
+        <v>45</v>
+      </c>
+      <c r="K7" t="s">
+        <v>51</v>
+      </c>
+      <c r="L7">
         <v>12</v>
       </c>
-      <c r="J7">
+      <c r="M7">
         <v>24</v>
       </c>
-      <c r="K7">
+      <c r="N7">
         <v>21</v>
       </c>
-      <c r="L7">
+      <c r="O7">
         <v>8</v>
       </c>
-      <c r="M7">
+      <c r="P7">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" s="1">
+        <v>129</v>
+      </c>
+      <c r="D8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" t="s">
+        <v>155</v>
+      </c>
+      <c r="F8" t="s">
+        <v>173</v>
+      </c>
+      <c r="G8" s="1">
         <v>44228</v>
       </c>
-      <c r="E8" s="5">
+      <c r="H8" s="5">
         <v>42.395432</v>
       </c>
-      <c r="F8" s="3">
+      <c r="I8" s="3">
         <v>-71.147199000000001</v>
       </c>
-      <c r="G8" t="s">
-        <v>48</v>
-      </c>
-      <c r="H8" t="s">
-        <v>65</v>
-      </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-      <c r="J8">
+      <c r="J8" t="s">
+        <v>45</v>
+      </c>
+      <c r="K8" t="s">
+        <v>51</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
         <v>15</v>
       </c>
-      <c r="K8">
+      <c r="N8">
         <v>13</v>
       </c>
-      <c r="L8">
+      <c r="O8">
         <v>21</v>
       </c>
-      <c r="M8">
+      <c r="P8">
         <v>6</v>
       </c>
-      <c r="N8" s="2"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="Q8" s="2"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" s="1">
+        <v>149</v>
+      </c>
+      <c r="D9" t="s">
+        <v>165</v>
+      </c>
+      <c r="E9" t="s">
+        <v>155</v>
+      </c>
+      <c r="F9" t="s">
+        <v>173</v>
+      </c>
+      <c r="G9" s="1">
         <v>44713</v>
       </c>
-      <c r="E9" s="5">
+      <c r="H9" s="5">
         <v>42.395432</v>
       </c>
-      <c r="F9" s="3">
+      <c r="I9" s="3">
         <v>-71.147199000000001</v>
       </c>
-      <c r="G9" t="s">
-        <v>48</v>
-      </c>
-      <c r="H9" t="s">
-        <v>65</v>
-      </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-      <c r="J9">
+      <c r="J9" t="s">
+        <v>45</v>
+      </c>
+      <c r="K9" t="s">
+        <v>51</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9">
         <v>5</v>
       </c>
-      <c r="K9">
+      <c r="N9">
         <v>8</v>
       </c>
-      <c r="L9">
+      <c r="O9">
         <v>17</v>
       </c>
-      <c r="M9">
+      <c r="P9">
         <v>25</v>
       </c>
-      <c r="N9" s="2"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="Q9" s="2"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" s="1">
+        <v>130</v>
+      </c>
+      <c r="D10" t="s">
+        <v>135</v>
+      </c>
+      <c r="E10" t="s">
+        <v>126</v>
+      </c>
+      <c r="F10" t="s">
+        <v>173</v>
+      </c>
+      <c r="G10" s="1">
         <v>44501</v>
       </c>
-      <c r="E10" s="5">
+      <c r="H10" s="5">
         <v>38.672257999999999</v>
       </c>
-      <c r="F10" s="3">
+      <c r="I10" s="3">
         <v>-90.489697000000007</v>
       </c>
-      <c r="G10" t="s">
-        <v>48</v>
-      </c>
-      <c r="H10" t="s">
-        <v>67</v>
-      </c>
-      <c r="I10">
+      <c r="J10" t="s">
+        <v>45</v>
+      </c>
+      <c r="K10" t="s">
+        <v>53</v>
+      </c>
+      <c r="L10">
         <v>6</v>
       </c>
-      <c r="J10">
+      <c r="M10">
         <v>11</v>
       </c>
-      <c r="K10">
+      <c r="N10">
         <v>25</v>
       </c>
-      <c r="L10">
+      <c r="O10">
         <v>22</v>
       </c>
-      <c r="M10">
+      <c r="P10">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="C11" t="s">
-        <v>132</v>
-      </c>
-      <c r="D11" s="1">
+        <v>149</v>
+      </c>
+      <c r="D11" t="s">
+        <v>166</v>
+      </c>
+      <c r="E11" t="s">
+        <v>117</v>
+      </c>
+      <c r="F11" t="s">
+        <v>173</v>
+      </c>
+      <c r="G11" s="1">
         <v>44828</v>
       </c>
-      <c r="E11" s="4">
+      <c r="H11" s="4">
         <v>42.864286999999997</v>
       </c>
-      <c r="F11" s="3">
+      <c r="I11" s="3">
         <v>-71.625247999999999</v>
       </c>
-      <c r="G11" t="s">
-        <v>100</v>
-      </c>
-      <c r="H11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I11">
-        <v>1</v>
-      </c>
-      <c r="J11">
+      <c r="J11" t="s">
+        <v>86</v>
+      </c>
+      <c r="K11" t="s">
+        <v>55</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11">
         <v>12</v>
       </c>
-      <c r="K11">
+      <c r="N11">
         <v>24</v>
       </c>
-      <c r="L11">
+      <c r="O11">
         <v>9</v>
       </c>
-      <c r="M11">
+      <c r="P11">
         <v>22</v>
       </c>
-      <c r="N11" s="2"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="Q11" s="2"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B12" t="s">
         <v>105</v>
       </c>
-      <c r="B12" t="s">
-        <v>120</v>
-      </c>
       <c r="C12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" s="1">
+        <v>129</v>
+      </c>
+      <c r="D12" t="s">
+        <v>136</v>
+      </c>
+      <c r="E12" t="s">
+        <v>151</v>
+      </c>
+      <c r="F12" t="s">
+        <v>173</v>
+      </c>
+      <c r="G12" s="1">
         <v>44774</v>
       </c>
-      <c r="E12" s="4">
+      <c r="H12" s="4">
         <v>42.486085000000003</v>
       </c>
-      <c r="F12" s="3">
+      <c r="I12" s="3">
         <v>-71.208479999999994</v>
       </c>
-      <c r="G12" t="s">
-        <v>48</v>
-      </c>
-      <c r="H12" t="s">
-        <v>65</v>
-      </c>
-      <c r="I12">
-        <v>1</v>
-      </c>
-      <c r="J12">
+      <c r="J12" t="s">
+        <v>45</v>
+      </c>
+      <c r="K12" t="s">
+        <v>51</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
         <v>4</v>
       </c>
-      <c r="K12">
+      <c r="N12">
         <v>13</v>
       </c>
-      <c r="L12">
+      <c r="O12">
         <v>11</v>
       </c>
-      <c r="M12">
+      <c r="P12">
         <v>16</v>
       </c>
-      <c r="N12" s="2"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="Q12" s="2"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
+        <v>161</v>
       </c>
       <c r="C13" t="s">
+        <v>129</v>
+      </c>
+      <c r="D13" t="s">
+        <v>137</v>
+      </c>
+      <c r="E13" t="s">
+        <v>156</v>
+      </c>
+      <c r="F13" t="s">
+        <v>173</v>
+      </c>
+      <c r="G13" s="1">
+        <v>44136</v>
+      </c>
+      <c r="H13" s="4">
+        <v>41.959066</v>
+      </c>
+      <c r="I13" s="3">
+        <v>-70.667964999999995</v>
+      </c>
+      <c r="J13" t="s">
+        <v>45</v>
+      </c>
+      <c r="K13" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="1">
-        <v>44136</v>
-      </c>
-      <c r="E13" s="4">
-        <v>41.959066</v>
-      </c>
-      <c r="F13" s="3">
-        <v>-70.667964999999995</v>
-      </c>
-      <c r="G13" t="s">
-        <v>48</v>
-      </c>
-      <c r="H13" t="s">
-        <v>65</v>
-      </c>
-      <c r="I13">
-        <v>1</v>
-      </c>
-      <c r="J13">
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="M13">
         <v>7</v>
       </c>
-      <c r="K13">
+      <c r="N13">
         <v>6</v>
       </c>
-      <c r="L13">
+      <c r="O13">
         <v>25</v>
       </c>
-      <c r="M13">
+      <c r="P13">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="C14" t="s">
-        <v>52</v>
-      </c>
-      <c r="D14" s="1">
+        <v>149</v>
+      </c>
+      <c r="D14" t="s">
+        <v>139</v>
+      </c>
+      <c r="E14" t="s">
+        <v>157</v>
+      </c>
+      <c r="F14" t="s">
+        <v>173</v>
+      </c>
+      <c r="G14" s="1">
         <v>43070</v>
       </c>
-      <c r="E14" s="4">
+      <c r="H14" s="4">
         <v>40.768414</v>
       </c>
-      <c r="F14" s="3">
+      <c r="I14" s="3">
         <v>-73.996746999999999</v>
       </c>
-      <c r="G14" t="s">
-        <v>48</v>
-      </c>
-      <c r="H14" t="s">
-        <v>65</v>
-      </c>
-      <c r="I14">
-        <v>1</v>
-      </c>
-      <c r="J14">
+      <c r="J14" t="s">
+        <v>45</v>
+      </c>
+      <c r="K14" t="s">
+        <v>51</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14">
         <v>5</v>
       </c>
-      <c r="K14">
+      <c r="N14">
         <v>16</v>
       </c>
-      <c r="L14">
+      <c r="O14">
         <v>22</v>
       </c>
-      <c r="M14">
-        <v>1</v>
-      </c>
-      <c r="N14" s="2"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P14">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="2"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
-      </c>
-      <c r="D15" s="1">
+        <v>129</v>
+      </c>
+      <c r="D15" t="s">
+        <v>138</v>
+      </c>
+      <c r="E15" t="s">
+        <v>157</v>
+      </c>
+      <c r="F15" t="s">
+        <v>173</v>
+      </c>
+      <c r="G15" s="1">
         <v>43435</v>
       </c>
-      <c r="E15" s="4">
+      <c r="H15" s="4">
         <v>40.689253000000001</v>
       </c>
-      <c r="F15" s="3">
+      <c r="I15" s="3">
         <v>-74.044548000000006</v>
       </c>
-      <c r="G15" t="s">
-        <v>48</v>
-      </c>
-      <c r="H15" t="s">
-        <v>65</v>
-      </c>
-      <c r="I15">
-        <v>1</v>
-      </c>
-      <c r="J15">
+      <c r="J15" t="s">
+        <v>45</v>
+      </c>
+      <c r="K15" t="s">
+        <v>51</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15">
         <v>6</v>
       </c>
-      <c r="K15">
+      <c r="N15">
         <v>8</v>
       </c>
-      <c r="L15">
+      <c r="O15">
         <v>18</v>
       </c>
-      <c r="M15">
+      <c r="P15">
         <v>8</v>
       </c>
-      <c r="N15" s="2"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="Q15" s="2"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C16" t="s">
-        <v>54</v>
-      </c>
-      <c r="D16" s="1">
+        <v>129</v>
+      </c>
+      <c r="D16" t="s">
+        <v>138</v>
+      </c>
+      <c r="E16" t="s">
+        <v>177</v>
+      </c>
+      <c r="F16" t="s">
+        <v>178</v>
+      </c>
+      <c r="G16" s="1">
         <v>43617</v>
       </c>
-      <c r="E16" s="4">
+      <c r="H16" s="4">
         <v>51.507322000000002</v>
       </c>
-      <c r="F16" s="3">
+      <c r="I16" s="3">
         <v>-0.12764700000000001</v>
       </c>
-      <c r="G16" t="s">
-        <v>48</v>
-      </c>
-      <c r="H16" t="s">
-        <v>65</v>
-      </c>
-      <c r="I16">
-        <v>1</v>
-      </c>
-      <c r="J16">
+      <c r="J16" t="s">
+        <v>45</v>
+      </c>
+      <c r="K16" t="s">
+        <v>51</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="M16">
         <v>11</v>
       </c>
-      <c r="K16">
+      <c r="N16">
         <v>4</v>
       </c>
-      <c r="L16">
+      <c r="O16">
         <v>19</v>
       </c>
-      <c r="M16">
+      <c r="P16">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
-      </c>
-      <c r="D17" s="1">
+        <v>129</v>
+      </c>
+      <c r="D17" t="s">
+        <v>131</v>
+      </c>
+      <c r="E17" t="s">
+        <v>175</v>
+      </c>
+      <c r="F17" t="s">
+        <v>42</v>
+      </c>
+      <c r="G17" s="1">
         <v>44682</v>
       </c>
-      <c r="E17" s="4">
+      <c r="H17" s="4">
         <v>32.074058999999998</v>
       </c>
-      <c r="F17" s="3">
+      <c r="I17" s="3">
         <v>34.775413</v>
       </c>
-      <c r="G17" t="s">
-        <v>48</v>
-      </c>
-      <c r="H17" t="s">
-        <v>65</v>
-      </c>
-      <c r="I17">
-        <v>1</v>
-      </c>
-      <c r="J17">
+      <c r="J17" t="s">
+        <v>45</v>
+      </c>
+      <c r="K17" t="s">
+        <v>51</v>
+      </c>
+      <c r="L17">
+        <v>1</v>
+      </c>
+      <c r="M17">
         <v>19</v>
       </c>
-      <c r="K17">
+      <c r="N17">
         <v>5</v>
       </c>
-      <c r="L17">
+      <c r="O17">
         <v>20</v>
       </c>
-      <c r="M17">
+      <c r="P17">
         <v>23</v>
       </c>
-      <c r="N17" s="2"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="Q17" s="2"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
-      </c>
-      <c r="D18" s="1">
+        <v>149</v>
+      </c>
+      <c r="D18" t="s">
+        <v>167</v>
+      </c>
+      <c r="E18" t="s">
+        <v>158</v>
+      </c>
+      <c r="F18" t="s">
+        <v>173</v>
+      </c>
+      <c r="G18" s="1">
         <v>44378</v>
       </c>
-      <c r="E18" s="4">
+      <c r="H18" s="4">
         <v>42.499966999999998</v>
       </c>
-      <c r="F18" s="3">
+      <c r="I18" s="3">
         <v>-70.854718000000005</v>
       </c>
-      <c r="G18" t="s">
-        <v>48</v>
-      </c>
-      <c r="H18" t="s">
-        <v>65</v>
-      </c>
-      <c r="I18">
-        <v>1</v>
-      </c>
-      <c r="J18">
+      <c r="J18" t="s">
+        <v>45</v>
+      </c>
+      <c r="K18" t="s">
+        <v>51</v>
+      </c>
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18">
         <v>11</v>
       </c>
-      <c r="K18">
+      <c r="N18">
         <v>22</v>
       </c>
-      <c r="L18">
+      <c r="O18">
         <v>8</v>
       </c>
-      <c r="M18">
+      <c r="P18">
         <v>4</v>
       </c>
-      <c r="N18" s="2"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="Q18" s="2"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="C19" t="s">
-        <v>56</v>
-      </c>
-      <c r="D19" s="1">
+        <v>129</v>
+      </c>
+      <c r="D19" t="s">
+        <v>140</v>
+      </c>
+      <c r="E19" t="s">
+        <v>179</v>
+      </c>
+      <c r="F19" t="s">
+        <v>46</v>
+      </c>
+      <c r="G19" s="1">
         <v>43252</v>
       </c>
-      <c r="E19" s="4">
+      <c r="H19" s="4">
         <v>41.383111999999997</v>
       </c>
-      <c r="F19" s="3">
+      <c r="I19" s="3">
         <v>2.1743480000000002</v>
       </c>
-      <c r="G19" t="s">
-        <v>48</v>
-      </c>
-      <c r="H19" t="s">
-        <v>68</v>
-      </c>
-      <c r="I19">
+      <c r="J19" t="s">
+        <v>45</v>
+      </c>
+      <c r="K19" t="s">
+        <v>54</v>
+      </c>
+      <c r="L19">
         <v>2</v>
       </c>
-      <c r="J19">
+      <c r="M19">
         <v>11</v>
       </c>
-      <c r="K19">
+      <c r="N19">
         <v>19</v>
       </c>
-      <c r="L19">
+      <c r="O19">
         <v>12</v>
       </c>
-      <c r="M19">
+      <c r="P19">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>115</v>
+        <v>164</v>
       </c>
       <c r="C20" t="s">
-        <v>46</v>
-      </c>
-      <c r="D20" s="1">
+        <v>130</v>
+      </c>
+      <c r="D20" t="s">
+        <v>141</v>
+      </c>
+      <c r="E20" t="s">
+        <v>155</v>
+      </c>
+      <c r="F20" t="s">
+        <v>173</v>
+      </c>
+      <c r="G20" s="1">
         <v>43977</v>
       </c>
-      <c r="E20" s="5">
+      <c r="H20" s="5">
         <v>42.395432</v>
       </c>
-      <c r="F20" s="3">
+      <c r="I20" s="3">
         <v>-71.147199000000001</v>
       </c>
-      <c r="G20" t="s">
-        <v>76</v>
-      </c>
-      <c r="H20" t="s">
-        <v>65</v>
-      </c>
-      <c r="I20">
-        <v>1</v>
-      </c>
-      <c r="J20">
+      <c r="J20" t="s">
+        <v>62</v>
+      </c>
+      <c r="K20" t="s">
+        <v>51</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="M20">
         <v>6</v>
       </c>
-      <c r="K20">
+      <c r="N20">
         <v>8</v>
       </c>
-      <c r="L20">
+      <c r="O20">
         <v>17</v>
       </c>
-      <c r="M20">
+      <c r="P20">
         <v>9</v>
       </c>
-      <c r="N20" s="2"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="Q20" s="2"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C21" t="s">
-        <v>43</v>
-      </c>
-      <c r="D21" s="1">
+        <v>129</v>
+      </c>
+      <c r="D21" t="s">
+        <v>131</v>
+      </c>
+      <c r="E21" t="s">
+        <v>175</v>
+      </c>
+      <c r="F21" t="s">
+        <v>42</v>
+      </c>
+      <c r="G21" s="1">
         <v>44682</v>
       </c>
-      <c r="E21" s="4">
+      <c r="H21" s="4">
         <v>32.074058999999998</v>
       </c>
-      <c r="F21" s="3">
+      <c r="I21" s="3">
         <v>34.775413</v>
       </c>
-      <c r="G21" t="s">
-        <v>48</v>
-      </c>
-      <c r="H21" t="s">
-        <v>65</v>
-      </c>
-      <c r="I21">
-        <v>1</v>
-      </c>
-      <c r="J21">
+      <c r="J21" t="s">
+        <v>45</v>
+      </c>
+      <c r="K21" t="s">
+        <v>51</v>
+      </c>
+      <c r="L21">
+        <v>1</v>
+      </c>
+      <c r="M21">
         <v>24</v>
       </c>
-      <c r="K21">
+      <c r="N21">
         <v>21</v>
       </c>
-      <c r="L21">
+      <c r="O21">
         <v>8</v>
       </c>
-      <c r="M21">
+      <c r="P21">
         <v>2</v>
       </c>
-      <c r="N21" s="2"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="Q21" s="2"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="C22" t="s">
-        <v>58</v>
-      </c>
-      <c r="D22" s="1">
+        <v>129</v>
+      </c>
+      <c r="D22" t="s">
+        <v>142</v>
+      </c>
+      <c r="E22" t="s">
+        <v>47</v>
+      </c>
+      <c r="F22" t="s">
+        <v>22</v>
+      </c>
+      <c r="G22" s="1">
         <v>44787</v>
       </c>
-      <c r="E22" s="4">
+      <c r="H22" s="4">
         <v>45.505358000000001</v>
       </c>
-      <c r="F22" s="3">
+      <c r="I22" s="3">
         <v>-73.554688999999996</v>
       </c>
-      <c r="G22" t="s">
-        <v>48</v>
-      </c>
-      <c r="H22" t="s">
-        <v>65</v>
-      </c>
-      <c r="I22">
-        <v>1</v>
-      </c>
-      <c r="J22">
+      <c r="J22" t="s">
+        <v>45</v>
+      </c>
+      <c r="K22" t="s">
+        <v>51</v>
+      </c>
+      <c r="L22">
+        <v>1</v>
+      </c>
+      <c r="M22">
         <v>11</v>
       </c>
-      <c r="K22">
+      <c r="N22">
         <v>12</v>
       </c>
-      <c r="L22">
+      <c r="O22">
         <v>25</v>
       </c>
-      <c r="M22">
+      <c r="P22">
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>37</v>
       </c>
       <c r="B23" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="C23" t="s">
-        <v>41</v>
-      </c>
-      <c r="D23" s="1">
+        <v>129</v>
+      </c>
+      <c r="D23" t="s">
+        <v>124</v>
+      </c>
+      <c r="E23" t="s">
+        <v>153</v>
+      </c>
+      <c r="F23" t="s">
+        <v>173</v>
+      </c>
+      <c r="G23" s="1">
         <v>43134</v>
       </c>
-      <c r="E23" s="4">
+      <c r="H23" s="4">
         <v>38.883940000000003</v>
       </c>
-      <c r="F23" s="3">
+      <c r="I23" s="3">
         <v>-77.025510999999995</v>
       </c>
-      <c r="G23" t="s">
-        <v>89</v>
-      </c>
-      <c r="H23" t="s">
-        <v>65</v>
-      </c>
-      <c r="I23">
-        <v>1</v>
-      </c>
-      <c r="J23">
+      <c r="J23" t="s">
+        <v>75</v>
+      </c>
+      <c r="K23" t="s">
+        <v>51</v>
+      </c>
+      <c r="L23">
+        <v>1</v>
+      </c>
+      <c r="M23">
         <v>22</v>
       </c>
-      <c r="K23">
+      <c r="N23">
         <v>10</v>
       </c>
-      <c r="L23">
+      <c r="O23">
         <v>11</v>
       </c>
-      <c r="M23">
+      <c r="P23">
         <v>13</v>
       </c>
-      <c r="N23" s="2"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="Q23" s="2"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="C24" t="s">
-        <v>57</v>
-      </c>
-      <c r="D24" s="1">
+        <v>129</v>
+      </c>
+      <c r="D24" t="s">
+        <v>143</v>
+      </c>
+      <c r="E24" t="s">
+        <v>159</v>
+      </c>
+      <c r="F24" t="s">
+        <v>173</v>
+      </c>
+      <c r="G24" s="1">
         <v>43101</v>
       </c>
-      <c r="E24" s="4">
+      <c r="H24" s="4">
         <v>28.450769999999999</v>
       </c>
-      <c r="F24" s="3">
+      <c r="I24" s="3">
         <v>-80.526619999999994</v>
       </c>
-      <c r="G24" t="s">
-        <v>86</v>
-      </c>
-      <c r="H24" t="s">
-        <v>65</v>
-      </c>
-      <c r="I24">
-        <v>1</v>
-      </c>
-      <c r="J24">
+      <c r="J24" t="s">
+        <v>72</v>
+      </c>
+      <c r="K24" t="s">
+        <v>51</v>
+      </c>
+      <c r="L24">
+        <v>1</v>
+      </c>
+      <c r="M24">
         <v>23</v>
       </c>
-      <c r="K24">
+      <c r="N24">
         <v>18</v>
       </c>
-      <c r="L24">
+      <c r="O24">
         <v>2</v>
       </c>
-      <c r="M24">
+      <c r="P24">
         <v>22</v>
       </c>
-      <c r="N24" s="2"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="Q24" s="2"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="C25" t="s">
-        <v>58</v>
-      </c>
-      <c r="D25" s="1">
+        <v>129</v>
+      </c>
+      <c r="D25" t="s">
+        <v>142</v>
+      </c>
+      <c r="E25" t="s">
+        <v>47</v>
+      </c>
+      <c r="F25" t="s">
+        <v>22</v>
+      </c>
+      <c r="G25" s="1">
         <v>44787</v>
       </c>
-      <c r="E25" s="4">
+      <c r="H25" s="4">
         <v>45.505358000000001</v>
       </c>
-      <c r="F25" s="3">
+      <c r="I25" s="3">
         <v>-73.554688999999996</v>
       </c>
-      <c r="G25" t="s">
-        <v>88</v>
-      </c>
-      <c r="H25" t="s">
-        <v>69</v>
-      </c>
-      <c r="I25">
-        <v>1</v>
-      </c>
-      <c r="J25">
-        <v>1</v>
-      </c>
-      <c r="K25">
+      <c r="J25" t="s">
+        <v>74</v>
+      </c>
+      <c r="K25" t="s">
+        <v>55</v>
+      </c>
+      <c r="L25">
+        <v>1</v>
+      </c>
+      <c r="M25">
+        <v>1</v>
+      </c>
+      <c r="N25">
         <v>12</v>
       </c>
-      <c r="L25">
+      <c r="O25">
         <v>15</v>
       </c>
-      <c r="M25">
+      <c r="P25">
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="C26" t="s">
-        <v>46</v>
-      </c>
-      <c r="D26" s="1">
+        <v>130</v>
+      </c>
+      <c r="D26" t="s">
+        <v>144</v>
+      </c>
+      <c r="E26" t="s">
+        <v>155</v>
+      </c>
+      <c r="F26" t="s">
+        <v>173</v>
+      </c>
+      <c r="G26" s="1">
         <v>44455</v>
       </c>
-      <c r="E26" s="5">
+      <c r="H26" s="5">
         <v>42.395432</v>
       </c>
-      <c r="F26" s="3">
+      <c r="I26" s="3">
         <v>-71.147199000000001</v>
       </c>
-      <c r="G26" t="s">
-        <v>48</v>
-      </c>
-      <c r="H26" t="s">
-        <v>65</v>
-      </c>
-      <c r="I26">
-        <v>1</v>
-      </c>
-      <c r="J26">
+      <c r="J26" t="s">
+        <v>45</v>
+      </c>
+      <c r="K26" t="s">
+        <v>51</v>
+      </c>
+      <c r="L26">
+        <v>1</v>
+      </c>
+      <c r="M26">
         <v>9</v>
       </c>
-      <c r="K26">
+      <c r="N26">
         <v>20</v>
       </c>
-      <c r="L26">
+      <c r="O26">
         <v>18</v>
       </c>
-      <c r="M26">
+      <c r="P26">
         <v>13</v>
       </c>
-      <c r="N26" s="2"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="Q26" s="2"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>24</v>
       </c>
       <c r="B27" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="C27" t="s">
-        <v>59</v>
-      </c>
-      <c r="D27" s="1">
+        <v>129</v>
+      </c>
+      <c r="D27" t="s">
+        <v>145</v>
+      </c>
+      <c r="E27" t="s">
+        <v>160</v>
+      </c>
+      <c r="F27" t="s">
+        <v>173</v>
+      </c>
+      <c r="G27" s="1">
         <v>43374</v>
       </c>
-      <c r="E27" s="4">
+      <c r="H27" s="4">
         <v>38.879098999999997</v>
       </c>
-      <c r="F27" s="3">
+      <c r="I27" s="3">
         <v>-77.111007000000001</v>
       </c>
-      <c r="G27" t="s">
-        <v>48</v>
-      </c>
-      <c r="H27" t="s">
-        <v>65</v>
-      </c>
-      <c r="I27">
-        <v>1</v>
-      </c>
-      <c r="J27">
+      <c r="J27" t="s">
+        <v>45</v>
+      </c>
+      <c r="K27" t="s">
+        <v>51</v>
+      </c>
+      <c r="L27">
+        <v>1</v>
+      </c>
+      <c r="M27">
         <v>25</v>
       </c>
-      <c r="K27">
+      <c r="N27">
         <v>23</v>
       </c>
-      <c r="L27">
+      <c r="O27">
         <v>10</v>
       </c>
-      <c r="M27">
+      <c r="P27">
         <v>12</v>
       </c>
-      <c r="N27" s="2"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="Q27" s="2"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="B28" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="C28" t="s">
-        <v>75</v>
-      </c>
-      <c r="D28" s="1">
+        <v>129</v>
+      </c>
+      <c r="D28" t="s">
+        <v>146</v>
+      </c>
+      <c r="E28" t="s">
+        <v>180</v>
+      </c>
+      <c r="F28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G28" s="1">
         <v>43617</v>
       </c>
-      <c r="E28" s="4">
+      <c r="H28" s="4">
         <v>48.208354</v>
       </c>
-      <c r="F28" s="3">
+      <c r="I28" s="3">
         <v>16.372503999999999</v>
       </c>
-      <c r="G28" t="s">
-        <v>48</v>
-      </c>
-      <c r="H28" t="s">
-        <v>70</v>
-      </c>
-      <c r="I28">
-        <v>1</v>
-      </c>
-      <c r="J28">
+      <c r="J28" t="s">
+        <v>45</v>
+      </c>
+      <c r="K28" t="s">
+        <v>56</v>
+      </c>
+      <c r="L28">
+        <v>1</v>
+      </c>
+      <c r="M28">
         <v>18</v>
       </c>
-      <c r="K28">
+      <c r="N28">
         <v>8</v>
       </c>
-      <c r="L28">
+      <c r="O28">
         <v>12</v>
       </c>
-      <c r="M28">
+      <c r="P28">
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C29" t="s">
-        <v>60</v>
-      </c>
-      <c r="D29" s="1">
+        <v>129</v>
+      </c>
+      <c r="D29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E29" t="s">
+        <v>153</v>
+      </c>
+      <c r="F29" t="s">
+        <v>173</v>
+      </c>
+      <c r="G29" s="1">
         <v>43617</v>
       </c>
-      <c r="E29" s="4">
+      <c r="H29" s="4">
         <v>38.851289000000001</v>
       </c>
-      <c r="F29" s="3">
+      <c r="I29" s="3">
         <v>-77.039688999999996</v>
       </c>
-      <c r="G29" t="s">
-        <v>48</v>
-      </c>
-      <c r="H29" t="s">
-        <v>65</v>
-      </c>
-      <c r="I29">
-        <v>1</v>
-      </c>
-      <c r="J29">
+      <c r="J29" t="s">
+        <v>45</v>
+      </c>
+      <c r="K29" t="s">
+        <v>51</v>
+      </c>
+      <c r="L29">
+        <v>1</v>
+      </c>
+      <c r="M29">
         <v>25</v>
       </c>
-      <c r="K29">
+      <c r="N29">
         <v>8</v>
       </c>
-      <c r="L29">
-        <v>1</v>
-      </c>
-      <c r="M29">
+      <c r="O29">
+        <v>1</v>
+      </c>
+      <c r="P29">
         <v>6</v>
       </c>
-      <c r="N29" s="2"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="Q29" s="2"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="C30" t="s">
-        <v>135</v>
-      </c>
-      <c r="D30" s="1">
+        <v>129</v>
+      </c>
+      <c r="D30" t="s">
+        <v>148</v>
+      </c>
+      <c r="E30" t="s">
+        <v>181</v>
+      </c>
+      <c r="F30" t="s">
+        <v>42</v>
+      </c>
+      <c r="G30" s="1">
         <v>44682</v>
       </c>
-      <c r="E30" s="4">
+      <c r="H30" s="4">
         <v>31.771888000000001</v>
       </c>
-      <c r="F30" s="3">
+      <c r="I30" s="3">
         <v>35.203386999999999</v>
       </c>
-      <c r="G30" t="s">
-        <v>48</v>
-      </c>
-      <c r="H30" t="s">
-        <v>65</v>
-      </c>
-      <c r="I30">
-        <v>1</v>
-      </c>
-      <c r="J30">
+      <c r="J30" t="s">
+        <v>45</v>
+      </c>
+      <c r="K30" t="s">
+        <v>51</v>
+      </c>
+      <c r="L30">
+        <v>1</v>
+      </c>
+      <c r="M30">
         <v>17</v>
       </c>
-      <c r="K30">
+      <c r="N30">
         <v>24</v>
       </c>
-      <c r="L30">
+      <c r="O30">
         <v>6</v>
       </c>
-      <c r="M30">
+      <c r="P30">
         <v>13</v>
       </c>
-      <c r="N30" s="2"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="Q30" s="2"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="C31" t="s">
-        <v>43</v>
-      </c>
-      <c r="D31" s="1">
+        <v>129</v>
+      </c>
+      <c r="D31" t="s">
+        <v>131</v>
+      </c>
+      <c r="E31" t="s">
+        <v>175</v>
+      </c>
+      <c r="F31" t="s">
+        <v>42</v>
+      </c>
+      <c r="G31" s="1">
         <v>44682</v>
       </c>
-      <c r="E31" s="4">
+      <c r="H31" s="4">
         <v>32.074058999999998</v>
       </c>
-      <c r="F31" s="3">
+      <c r="I31" s="3">
         <v>34.775413</v>
       </c>
-      <c r="G31" t="s">
-        <v>48</v>
-      </c>
-      <c r="H31" t="s">
-        <v>65</v>
-      </c>
-      <c r="I31">
-        <v>1</v>
-      </c>
-      <c r="J31">
+      <c r="J31" t="s">
+        <v>45</v>
+      </c>
+      <c r="K31" t="s">
+        <v>51</v>
+      </c>
+      <c r="L31">
+        <v>1</v>
+      </c>
+      <c r="M31">
         <v>15</v>
       </c>
-      <c r="K31">
+      <c r="N31">
         <v>24</v>
       </c>
-      <c r="L31">
+      <c r="O31">
         <v>12</v>
       </c>
-      <c r="M31">
+      <c r="P31">
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>29</v>
       </c>
       <c r="B32" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="C32" t="s">
-        <v>46</v>
-      </c>
-      <c r="D32" s="1">
+        <v>130</v>
+      </c>
+      <c r="D32" t="s">
+        <v>141</v>
+      </c>
+      <c r="E32" t="s">
+        <v>155</v>
+      </c>
+      <c r="F32" t="s">
+        <v>173</v>
+      </c>
+      <c r="G32" s="1">
         <v>43977</v>
       </c>
-      <c r="E32" s="5">
+      <c r="H32" s="5">
         <v>42.395432</v>
       </c>
-      <c r="F32" s="3">
+      <c r="I32" s="3">
         <v>-71.147199000000001</v>
       </c>
-      <c r="G32" t="s">
-        <v>48</v>
-      </c>
-      <c r="H32" t="s">
-        <v>65</v>
-      </c>
-      <c r="I32">
-        <v>1</v>
-      </c>
-      <c r="J32">
+      <c r="J32" t="s">
+        <v>45</v>
+      </c>
+      <c r="K32" t="s">
+        <v>51</v>
+      </c>
+      <c r="L32">
+        <v>1</v>
+      </c>
+      <c r="M32">
         <v>5</v>
       </c>
-      <c r="K32">
+      <c r="N32">
         <v>3</v>
       </c>
-      <c r="L32">
+      <c r="O32">
         <v>11</v>
       </c>
-      <c r="M32">
+      <c r="P32">
         <v>24</v>
       </c>
-      <c r="N32" s="2"/>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="Q32" s="2"/>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>30</v>
       </c>
       <c r="B33" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="C33" t="s">
-        <v>61</v>
-      </c>
-      <c r="D33" s="1">
+        <v>149</v>
+      </c>
+      <c r="D33" t="s">
+        <v>168</v>
+      </c>
+      <c r="E33" t="s">
+        <v>152</v>
+      </c>
+      <c r="F33" t="s">
+        <v>173</v>
+      </c>
+      <c r="G33" s="1">
         <v>44805</v>
       </c>
-      <c r="E33" s="4">
+      <c r="H33" s="4">
         <v>42.522596</v>
       </c>
-      <c r="F33" s="3">
+      <c r="I33" s="3">
         <v>-70.892773000000005</v>
       </c>
-      <c r="G33" t="s">
-        <v>127</v>
-      </c>
-      <c r="H33" t="s">
-        <v>65</v>
-      </c>
-      <c r="I33">
-        <v>1</v>
-      </c>
-      <c r="J33">
+      <c r="J33" t="s">
+        <v>112</v>
+      </c>
+      <c r="K33" t="s">
+        <v>51</v>
+      </c>
+      <c r="L33">
+        <v>1</v>
+      </c>
+      <c r="M33">
         <v>22</v>
       </c>
-      <c r="K33">
+      <c r="N33">
         <v>25</v>
       </c>
-      <c r="L33">
+      <c r="O33">
         <v>17</v>
       </c>
-      <c r="M33">
+      <c r="P33">
         <v>13</v>
       </c>
-      <c r="N33" s="2"/>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="Q33" s="2"/>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="C34" t="s">
-        <v>62</v>
-      </c>
-      <c r="D34" s="1">
+        <v>169</v>
+      </c>
+      <c r="D34" t="s">
+        <v>48</v>
+      </c>
+      <c r="E34" t="s">
+        <v>176</v>
+      </c>
+      <c r="F34" t="s">
+        <v>173</v>
+      </c>
+      <c r="G34" s="1">
         <v>42795</v>
       </c>
-      <c r="E34" s="4">
+      <c r="H34" s="4">
         <v>40.444902999999996</v>
       </c>
-      <c r="F34" s="3">
+      <c r="I34" s="3">
         <v>-79.942740999999998</v>
       </c>
-      <c r="G34" t="s">
-        <v>48</v>
-      </c>
-      <c r="H34" t="s">
-        <v>65</v>
-      </c>
-      <c r="I34">
-        <v>1</v>
-      </c>
-      <c r="J34">
+      <c r="J34" t="s">
+        <v>45</v>
+      </c>
+      <c r="K34" t="s">
+        <v>51</v>
+      </c>
+      <c r="L34">
+        <v>1</v>
+      </c>
+      <c r="M34">
         <v>14</v>
       </c>
-      <c r="K34">
+      <c r="N34">
         <v>6</v>
       </c>
-      <c r="L34">
+      <c r="O34">
         <v>15</v>
       </c>
-      <c r="M34">
+      <c r="P34">
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="C35" t="s">
-        <v>41</v>
-      </c>
-      <c r="D35" s="1">
+        <v>129</v>
+      </c>
+      <c r="D35" t="s">
+        <v>124</v>
+      </c>
+      <c r="E35" t="s">
+        <v>153</v>
+      </c>
+      <c r="F35" t="s">
+        <v>173</v>
+      </c>
+      <c r="G35" s="1">
         <v>43134</v>
       </c>
-      <c r="E35" s="4">
+      <c r="H35" s="4">
         <v>38.883940000000003</v>
       </c>
-      <c r="F35" s="3">
+      <c r="I35" s="3">
         <v>-77.025510999999995</v>
       </c>
-      <c r="G35" t="s">
-        <v>48</v>
-      </c>
-      <c r="H35" t="s">
-        <v>65</v>
-      </c>
-      <c r="I35">
-        <v>1</v>
-      </c>
-      <c r="J35">
+      <c r="J35" t="s">
+        <v>45</v>
+      </c>
+      <c r="K35" t="s">
+        <v>51</v>
+      </c>
+      <c r="L35">
+        <v>1</v>
+      </c>
+      <c r="M35">
         <v>23</v>
       </c>
-      <c r="K35">
+      <c r="N35">
         <v>17</v>
       </c>
-      <c r="L35">
+      <c r="O35">
         <v>25</v>
       </c>
-      <c r="M35">
+      <c r="P35">
         <v>20</v>
       </c>
-      <c r="N35" s="2"/>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="Q35" s="2"/>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>33</v>
       </c>
       <c r="B36" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="C36" t="s">
-        <v>133</v>
-      </c>
-      <c r="D36" s="1">
+        <v>149</v>
+      </c>
+      <c r="D36" t="s">
+        <v>170</v>
+      </c>
+      <c r="E36" t="s">
+        <v>152</v>
+      </c>
+      <c r="F36" t="s">
+        <v>173</v>
+      </c>
+      <c r="G36" s="1">
         <v>44803</v>
       </c>
-      <c r="E36" s="4">
+      <c r="H36" s="4">
         <v>42.522075000000001</v>
       </c>
-      <c r="F36" s="3">
+      <c r="I36" s="3">
         <v>-70.895891000000006</v>
       </c>
-      <c r="G36" t="s">
-        <v>48</v>
-      </c>
-      <c r="H36" t="s">
-        <v>65</v>
-      </c>
-      <c r="I36">
-        <v>1</v>
-      </c>
-      <c r="J36">
+      <c r="J36" t="s">
+        <v>45</v>
+      </c>
+      <c r="K36" t="s">
+        <v>51</v>
+      </c>
+      <c r="L36">
+        <v>1</v>
+      </c>
+      <c r="M36">
         <v>25</v>
       </c>
-      <c r="K36">
+      <c r="N36">
         <v>3</v>
       </c>
-      <c r="L36">
+      <c r="O36">
         <v>12</v>
       </c>
-      <c r="M36">
+      <c r="P36">
         <v>2</v>
       </c>
-      <c r="N36" s="2"/>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="Q36" s="2"/>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>34</v>
       </c>
       <c r="B37" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C37" t="s">
-        <v>133</v>
-      </c>
-      <c r="D37" s="1">
+        <v>149</v>
+      </c>
+      <c r="D37" t="s">
+        <v>170</v>
+      </c>
+      <c r="E37" t="s">
+        <v>152</v>
+      </c>
+      <c r="F37" t="s">
+        <v>173</v>
+      </c>
+      <c r="G37" s="1">
         <v>44762</v>
       </c>
-      <c r="E37" s="4">
+      <c r="H37" s="4">
         <v>42.522075000000001</v>
       </c>
-      <c r="F37" s="3">
+      <c r="I37" s="3">
         <v>-70.895891000000006</v>
       </c>
-      <c r="G37" t="s">
-        <v>48</v>
-      </c>
-      <c r="H37" t="s">
-        <v>65</v>
-      </c>
-      <c r="I37">
-        <v>1</v>
-      </c>
-      <c r="J37">
+      <c r="J37" t="s">
+        <v>45</v>
+      </c>
+      <c r="K37" t="s">
+        <v>51</v>
+      </c>
+      <c r="L37">
+        <v>1</v>
+      </c>
+      <c r="M37">
         <v>7</v>
       </c>
-      <c r="K37">
+      <c r="N37">
         <v>14</v>
       </c>
-      <c r="L37">
+      <c r="O37">
         <v>10</v>
       </c>
-      <c r="M37">
+      <c r="P37">
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="C38" t="s">
-        <v>132</v>
-      </c>
-      <c r="D38" s="1">
+        <v>149</v>
+      </c>
+      <c r="D38" t="s">
+        <v>166</v>
+      </c>
+      <c r="E38" t="s">
+        <v>117</v>
+      </c>
+      <c r="F38" t="s">
+        <v>173</v>
+      </c>
+      <c r="G38" s="1">
         <v>44829</v>
       </c>
-      <c r="E38" s="4">
+      <c r="H38" s="4">
         <v>42.864286999999997</v>
       </c>
-      <c r="F38" s="3">
+      <c r="I38" s="3">
         <v>-71.625247999999999</v>
       </c>
-      <c r="G38" t="s">
-        <v>48</v>
-      </c>
-      <c r="H38" t="s">
-        <v>69</v>
-      </c>
-      <c r="I38">
-        <v>1</v>
-      </c>
-      <c r="J38">
+      <c r="J38" t="s">
+        <v>45</v>
+      </c>
+      <c r="K38" t="s">
+        <v>55</v>
+      </c>
+      <c r="L38">
+        <v>1</v>
+      </c>
+      <c r="M38">
         <v>13</v>
       </c>
-      <c r="K38">
+      <c r="N38">
         <v>22</v>
       </c>
-      <c r="L38">
+      <c r="O38">
         <v>14</v>
       </c>
-      <c r="M38">
+      <c r="P38">
         <v>10</v>
       </c>
-      <c r="N38" s="2"/>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="Q38" s="2"/>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="B39" t="s">
-        <v>48</v>
+        <v>162</v>
       </c>
       <c r="C39" t="s">
-        <v>48</v>
-      </c>
-      <c r="D39" s="1">
+        <v>129</v>
+      </c>
+      <c r="D39" t="s">
+        <v>150</v>
+      </c>
+      <c r="E39" t="s">
+        <v>151</v>
+      </c>
+      <c r="F39" t="s">
+        <v>173</v>
+      </c>
+      <c r="G39" s="1">
         <v>44872</v>
       </c>
-      <c r="E39" s="4">
+      <c r="H39" s="4">
         <v>42.495154999999997</v>
       </c>
-      <c r="F39" s="3">
+      <c r="I39" s="3">
         <v>-71.191412</v>
       </c>
-      <c r="G39" t="s">
-        <v>48</v>
-      </c>
-      <c r="H39" t="s">
-        <v>124</v>
-      </c>
-      <c r="I39">
-        <v>1</v>
-      </c>
-      <c r="J39">
-        <v>1</v>
-      </c>
-      <c r="K39">
+      <c r="J39" t="s">
+        <v>45</v>
+      </c>
+      <c r="K39" t="s">
+        <v>109</v>
+      </c>
+      <c r="L39">
+        <v>1</v>
+      </c>
+      <c r="M39">
+        <v>1</v>
+      </c>
+      <c r="N39">
         <v>7</v>
       </c>
-      <c r="L39">
+      <c r="O39">
         <v>3</v>
       </c>
-      <c r="M39">
-        <v>1</v>
-      </c>
-      <c r="N39" s="2"/>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P39">
+        <v>1</v>
+      </c>
+      <c r="Q39" s="2"/>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="B40" t="s">
-        <v>48</v>
+        <v>163</v>
       </c>
       <c r="C40" t="s">
-        <v>48</v>
-      </c>
-      <c r="D40" s="1">
+        <v>129</v>
+      </c>
+      <c r="D40" t="s">
+        <v>150</v>
+      </c>
+      <c r="E40" t="s">
+        <v>151</v>
+      </c>
+      <c r="F40" t="s">
+        <v>173</v>
+      </c>
+      <c r="G40" s="1">
         <v>44872</v>
       </c>
-      <c r="E40" s="4">
+      <c r="H40" s="4">
         <v>42.495154999999997</v>
       </c>
-      <c r="F40" s="3">
+      <c r="I40" s="3">
         <v>-71.191412</v>
       </c>
-      <c r="G40" t="s">
-        <v>48</v>
-      </c>
-      <c r="H40" t="s">
-        <v>124</v>
-      </c>
-      <c r="I40">
-        <v>1</v>
-      </c>
-      <c r="J40">
+      <c r="J40" t="s">
+        <v>45</v>
+      </c>
+      <c r="K40" t="s">
+        <v>109</v>
+      </c>
+      <c r="L40">
+        <v>1</v>
+      </c>
+      <c r="M40">
         <v>13</v>
       </c>
-      <c r="K40">
+      <c r="N40">
         <v>22</v>
       </c>
-      <c r="L40">
+      <c r="O40">
         <v>14</v>
       </c>
-      <c r="M40">
+      <c r="P40">
         <v>3</v>
       </c>
     </row>
@@ -2626,10 +3106,10 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="B1" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="C1" t="s">
         <v>38</v>
@@ -2641,21 +3121,21 @@
         <v>39</v>
       </c>
       <c r="F1" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="G1" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="H1" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="I1" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="D2" s="1"/>
     </row>
@@ -2664,13 +3144,13 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D3" s="1">
         <v>44835</v>
       </c>
       <c r="F3" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -2681,13 +3161,13 @@
         <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D4" s="1">
         <v>44835</v>
       </c>
       <c r="F4" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -2695,43 +3175,43 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="D11" s="1"/>
     </row>

</xml_diff>

<commit_message>
added pie chart and re-formatted
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\Documents\DS_Projects\Analyducks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F607FA12-D896-4867-9E52-580050D79AB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2FE9DFD-34C7-4625-B13F-153188146C46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EF9DEEC2-186D-4161-AB80-57C24753F6AE}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="198">
   <si>
     <t>Duck</t>
   </si>
@@ -628,6 +628,9 @@
   </si>
   <si>
     <t>PA</t>
+  </si>
+  <si>
+    <t>QC</t>
   </si>
 </sst>
 </file>
@@ -1076,8 +1079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B28BE0B7-C424-43DE-B13E-D21D7F7285C7}">
   <dimension ref="A1:S40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="114" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="114" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2282,6 +2285,9 @@
       <c r="E22" t="s">
         <v>47</v>
       </c>
+      <c r="F22" t="s">
+        <v>197</v>
+      </c>
       <c r="G22" t="s">
         <v>22</v>
       </c>
@@ -2449,6 +2455,9 @@
       <c r="E25" t="s">
         <v>47</v>
       </c>
+      <c r="F25" t="s">
+        <v>197</v>
+      </c>
       <c r="G25" t="s">
         <v>22</v>
       </c>
@@ -3222,7 +3231,7 @@
         <v>161</v>
       </c>
       <c r="C39" t="s">
-        <v>128</v>
+        <v>108</v>
       </c>
       <c r="D39" t="s">
         <v>149</v>
@@ -3279,7 +3288,7 @@
         <v>162</v>
       </c>
       <c r="C40" t="s">
-        <v>128</v>
+        <v>108</v>
       </c>
       <c r="D40" t="s">
         <v>149</v>

</xml_diff>

<commit_message>
playing with map styling
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\Documents\DS_Projects\Analyducks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2FE9DFD-34C7-4625-B13F-153188146C46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{923B7F51-5D0C-4ACB-AEF9-B2E48E2A22F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EF9DEEC2-186D-4161-AB80-57C24753F6AE}"/>
   </bookViews>
@@ -1079,8 +1079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B28BE0B7-C424-43DE-B13E-D21D7F7285C7}">
   <dimension ref="A1:S40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="114" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="H20" zoomScale="114" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="O34" sqref="O34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3261,7 +3261,7 @@
         <v>45</v>
       </c>
       <c r="M39" t="s">
-        <v>108</v>
+        <v>51</v>
       </c>
       <c r="N39">
         <v>1</v>
@@ -3318,7 +3318,7 @@
         <v>45</v>
       </c>
       <c r="M40" t="s">
-        <v>108</v>
+        <v>51</v>
       </c>
       <c r="N40">
         <v>1</v>

</xml_diff>

<commit_message>
modifying the fact data
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\Documents\DS_Projects\Analyducks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41573969-7EF8-49F1-BD4C-B29EEB16D6FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33FFB533-97EA-411D-B208-6863C229B0DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EF9DEEC2-186D-4161-AB80-57C24753F6AE}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="216">
   <si>
     <t>Duck</t>
   </si>
@@ -597,9 +597,6 @@
     <t>I graduated top of my flock at Carnegie Mallard University, majoring in Mequacknical Engineering.</t>
   </si>
   <si>
-    <t>Trick or treat, smell my feet, give me something good to eat, if you don't I won't care, I'll just pull up your underwear.</t>
-  </si>
-  <si>
     <t>Give me your tired, your poor, Your huddled masses yearning to fly free, The wretched refuse of your teeming shore.</t>
   </si>
   <si>
@@ -648,9 +645,6 @@
     <t>We're up all night to get ducky 🦆</t>
   </si>
   <si>
-    <t>The Donald</t>
-  </si>
-  <si>
     <t>I will use my one wing to rule them all.</t>
   </si>
   <si>
@@ -664,6 +658,39 @@
   </si>
   <si>
     <t>When I'm not at Cape CaQuackeral, I love orbiting on the Space Shuttle Duckscovery.</t>
+  </si>
+  <si>
+    <t>I'm 50% mermaid, 50% duck, and 100% that billtch</t>
+  </si>
+  <si>
+    <t>I love long walks in the Fowlbidden Forest, one time I even saw Ron Webbsley!</t>
+  </si>
+  <si>
+    <t>Finding the Ark of the Covenant and the Holy Quail is all in a day's work for me.</t>
+  </si>
+  <si>
+    <t>Backquaker</t>
+  </si>
+  <si>
+    <t>My hat's propeller makes my migrations a kaleidoscope of color!</t>
+  </si>
+  <si>
+    <t>Trick or treat, smell our beaks, give us something good to eat, if you don't we won't care, we'll just pull up your underwear.</t>
+  </si>
+  <si>
+    <t>I want to become a Pokemon like my big bro Porygon. My signature move is Printed Peck Attack.</t>
+  </si>
+  <si>
+    <t>Don't tell Jack, but I'm the real pumpkin king.</t>
+  </si>
+  <si>
+    <t>If I were a rich duck.
+Ya ba dibba dibba dibba dibba dibba dibba dum
+All day long, I'd biddy biddy bum.
+If I were a wealthy duck
+I wouldn't have to fly hard
+Ya ba dibba dibba dibba dibba dibba dibba dum.
+If I were a biddy biddy rich yidle-diddle-didle-didle duck</t>
   </si>
 </sst>
 </file>
@@ -743,7 +770,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -757,6 +784,9 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -793,9 +823,6 @@
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -821,10 +848,10 @@
     <tableColumn id="18" xr3:uid="{6CF5BE57-FA6C-4A82-BBEB-02BD6F0FF1A7}" name="Purchase_State"/>
     <tableColumn id="16" xr3:uid="{8F6D77DD-9950-4A0C-9650-EF78F2440AF5}" name="Purchase_Country"/>
     <tableColumn id="17" xr3:uid="{53E3F17B-A5D5-4AE9-83A1-0970087FA2AC}" name="ISO_Code"/>
-    <tableColumn id="4" xr3:uid="{3483BEC1-7940-46EA-87AB-895F2A60F5C4}" name="Date_Bought" dataDxfId="3"/>
-    <tableColumn id="14" xr3:uid="{DD5702CA-A5AA-48F2-A221-5B11E7770312}" name="Latitude" dataDxfId="2"/>
-    <tableColumn id="13" xr3:uid="{6E84405B-586B-45AE-8AAB-E75DDE55DE14}" name="Longitude" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{D54F7BD0-C645-4075-B34E-4D059919801A}" name="About Me/Fun Fact" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{3483BEC1-7940-46EA-87AB-895F2A60F5C4}" name="Date_Bought" dataDxfId="4"/>
+    <tableColumn id="14" xr3:uid="{DD5702CA-A5AA-48F2-A221-5B11E7770312}" name="Latitude" dataDxfId="3"/>
+    <tableColumn id="13" xr3:uid="{6E84405B-586B-45AE-8AAB-E75DDE55DE14}" name="Longitude" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{D54F7BD0-C645-4075-B34E-4D059919801A}" name="About Me/Fun Fact" dataDxfId="1"/>
     <tableColumn id="6" xr3:uid="{E6929EE2-9995-48C5-99C7-C33245F8F30B}" name="Buyer"/>
     <tableColumn id="8" xr3:uid="{291141F9-BF51-4E10-B8D7-FD40E791433E}" name="Quantity"/>
     <tableColumn id="9" xr3:uid="{B5508D8E-FAD5-4D52-8444-0DB243E6A995}" name="Total_Weight"/>
@@ -843,7 +870,7 @@
     <tableColumn id="1" xr3:uid="{9E64D190-0A43-40CF-AD36-FD04A662496B}" name="Cousins"/>
     <tableColumn id="2" xr3:uid="{B24B008B-4FA5-4F53-8DFF-6B5E687E43FD}" name="Description"/>
     <tableColumn id="3" xr3:uid="{D04918B6-CEB1-4249-B203-04B49B77C2DB}" name="Location bought"/>
-    <tableColumn id="4" xr3:uid="{3D940517-F53B-4DDA-9410-4146A9DBC72B}" name="Date Bought" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{3D940517-F53B-4DDA-9410-4146A9DBC72B}" name="Date Bought" dataDxfId="0"/>
     <tableColumn id="5" xr3:uid="{51611A3A-347A-410D-87A5-C3B9A034AE16}" name="Fun Fact?"/>
     <tableColumn id="6" xr3:uid="{148B1608-FB51-4737-AD44-B59CA6A1087F}" name="Bought By"/>
     <tableColumn id="7" xr3:uid="{F988032F-024C-44D8-A1BB-16110E5DAE33}" name="Catch Phrase"/>
@@ -1153,9 +1180,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B28BE0B7-C424-43DE-B13E-D21D7F7285C7}">
   <dimension ref="A1:S40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="114" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="114" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="2" topLeftCell="K1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L32" sqref="L32"/>
+      <selection pane="topRight" activeCell="L44" sqref="L44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1211,7 +1238,7 @@
         <v>105</v>
       </c>
       <c r="L1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="M1" t="s">
         <v>107</v>
@@ -1267,7 +1294,7 @@
         <v>-77.025510999999995</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="M2" t="s">
         <v>51</v>
@@ -1321,7 +1348,7 @@
         <v>2.340983</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="M3" t="s">
         <v>52</v>
@@ -1375,7 +1402,7 @@
         <v>34.775413</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="M4" t="s">
         <v>51</v>
@@ -1431,7 +1458,7 @@
         <v>-73.846541999999999</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="M5" t="s">
         <v>51</v>
@@ -1515,7 +1542,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C7" t="s">
         <v>115</v>
@@ -1545,7 +1572,7 @@
         <v>-77.089934999999997</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M7" t="s">
         <v>51</v>
@@ -1601,7 +1628,7 @@
         <v>-71.147199000000001</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="M8" t="s">
         <v>51</v>
@@ -1658,7 +1685,7 @@
         <v>-71.147199000000001</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="M9" t="s">
         <v>51</v>
@@ -1714,8 +1741,8 @@
       <c r="K10" s="4">
         <v>-90.489697000000007</v>
       </c>
-      <c r="L10" s="7" t="s">
-        <v>186</v>
+      <c r="L10" s="6" t="s">
+        <v>212</v>
       </c>
       <c r="M10" t="s">
         <v>53</v>
@@ -1906,7 +1933,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1935,13 +1962,13 @@
         <v>43070</v>
       </c>
       <c r="J14" s="3">
-        <v>40.768414</v>
+        <v>40.769410000000001</v>
       </c>
       <c r="K14" s="4">
-        <v>-73.996746999999999</v>
+        <v>-73.996311000000006</v>
       </c>
       <c r="L14" s="6" t="s">
-        <v>45</v>
+        <v>211</v>
       </c>
       <c r="M14" t="s">
         <v>51</v>
@@ -1992,13 +2019,13 @@
         <v>43435</v>
       </c>
       <c r="J15" s="3">
-        <v>40.689253000000001</v>
+        <v>40.689183999999997</v>
       </c>
       <c r="K15" s="4">
-        <v>-74.044548000000006</v>
+        <v>-74.044769000000002</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="M15" t="s">
         <v>51</v>
@@ -2052,7 +2079,7 @@
         <v>-0.12764700000000001</v>
       </c>
       <c r="L16" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="M16" t="s">
         <v>51</v>
@@ -2127,7 +2154,7 @@
       </c>
       <c r="S17" s="2"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -2162,7 +2189,7 @@
         <v>-70.854718000000005</v>
       </c>
       <c r="L18" s="6" t="s">
-        <v>45</v>
+        <v>207</v>
       </c>
       <c r="M18" t="s">
         <v>51</v>
@@ -2216,7 +2243,7 @@
         <v>2.1743480000000002</v>
       </c>
       <c r="L19" s="6" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="M19" t="s">
         <v>54</v>
@@ -2272,7 +2299,7 @@
         <v>-71.147199000000001</v>
       </c>
       <c r="L20" s="6" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="M20" t="s">
         <v>51</v>
@@ -2326,7 +2353,7 @@
         <v>34.775413</v>
       </c>
       <c r="L21" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="M21" t="s">
         <v>51</v>
@@ -2383,7 +2410,7 @@
         <v>-73.554688999999996</v>
       </c>
       <c r="L22" s="6" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="M22" t="s">
         <v>51</v>
@@ -2439,7 +2466,7 @@
         <v>-77.025510999999995</v>
       </c>
       <c r="L23" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="M23" t="s">
         <v>51</v>
@@ -2496,7 +2523,7 @@
         <v>-80.526619999999994</v>
       </c>
       <c r="L24" s="6" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="M24" t="s">
         <v>51</v>
@@ -2553,7 +2580,7 @@
         <v>-73.554688999999996</v>
       </c>
       <c r="L25" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="M25" t="s">
         <v>55</v>
@@ -2574,7 +2601,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -2609,7 +2636,7 @@
         <v>-71.147199000000001</v>
       </c>
       <c r="L26" s="6" t="s">
-        <v>45</v>
+        <v>213</v>
       </c>
       <c r="M26" t="s">
         <v>51</v>
@@ -2666,7 +2693,7 @@
         <v>-77.111007000000001</v>
       </c>
       <c r="L27" s="6" t="s">
-        <v>45</v>
+        <v>214</v>
       </c>
       <c r="M27" t="s">
         <v>51</v>
@@ -2746,7 +2773,7 @@
         <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="C29" t="s">
         <v>114</v>
@@ -2798,7 +2825,7 @@
       </c>
       <c r="S29" s="2"/>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>27</v>
       </c>
@@ -2830,7 +2857,7 @@
         <v>35.203386999999999</v>
       </c>
       <c r="L30" s="6" t="s">
-        <v>45</v>
+        <v>215</v>
       </c>
       <c r="M30" t="s">
         <v>51</v>
@@ -2852,7 +2879,7 @@
       </c>
       <c r="S30" s="2"/>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>28</v>
       </c>
@@ -2884,7 +2911,7 @@
         <v>34.775413</v>
       </c>
       <c r="L31" s="6" t="s">
-        <v>45</v>
+        <v>209</v>
       </c>
       <c r="M31" t="s">
         <v>51</v>
@@ -2997,7 +3024,7 @@
         <v>-70.892773000000005</v>
       </c>
       <c r="L33" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M33" t="s">
         <v>51</v>
@@ -3110,7 +3137,7 @@
         <v>-77.025510999999995</v>
       </c>
       <c r="L35" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M35" t="s">
         <v>51</v>
@@ -3250,7 +3277,7 @@
         <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C38" t="s">
         <v>134</v>
@@ -3359,7 +3386,7 @@
       </c>
       <c r="S39" s="2"/>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>99</v>
       </c>
@@ -3394,7 +3421,7 @@
         <v>-71.191412</v>
       </c>
       <c r="L40" s="6" t="s">
-        <v>45</v>
+        <v>208</v>
       </c>
       <c r="M40" t="s">
         <v>51</v>

</xml_diff>

<commit_message>
added new duck data
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\Documents\DS_Projects\Analyducks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{728A7F40-CA83-412A-8F21-CEA0A6E0B371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{408E2009-BD6F-44D0-A66B-03B2C5317C63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EF9DEEC2-186D-4161-AB80-57C24753F6AE}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="232">
   <si>
     <t>Duck</t>
   </si>
@@ -751,6 +751,15 @@
 I wouldn't have to fly hard
 Ya ba dibba dibba dibba dibba dibba dibba dum.
 If I were a biddy biddy rich yidle-diddle-didle-didle duck.</t>
+  </si>
+  <si>
+    <t>Strawberry</t>
+  </si>
+  <si>
+    <t>Unicorn Large</t>
+  </si>
+  <si>
+    <t>Target</t>
   </si>
 </sst>
 </file>
@@ -823,7 +832,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -833,6 +842,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -892,8 +902,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{55715085-9AFB-4516-817F-DC3F49C2B133}" name="Table1" displayName="Table1" ref="A1:R40" totalsRowShown="0">
-  <autoFilter ref="A1:R40" xr:uid="{55715085-9AFB-4516-817F-DC3F49C2B133}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{55715085-9AFB-4516-817F-DC3F49C2B133}" name="Table1" displayName="Table1" ref="A1:R42" totalsRowShown="0">
+  <autoFilter ref="A1:R42" xr:uid="{55715085-9AFB-4516-817F-DC3F49C2B133}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R40">
     <sortCondition ref="B1:B40"/>
   </sortState>
@@ -1236,11 +1246,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B28BE0B7-C424-43DE-B13E-D21D7F7285C7}">
-  <dimension ref="A1:V40"/>
+  <dimension ref="A1:V42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="125" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L30" sqref="L30"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="125" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="K1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="L43" sqref="L43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3502,6 +3512,108 @@
       </c>
       <c r="R40">
         <v>9.6999999999999993</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>229</v>
+      </c>
+      <c r="C41" t="s">
+        <v>112</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="E41" t="s">
+        <v>178</v>
+      </c>
+      <c r="F41" t="s">
+        <v>163</v>
+      </c>
+      <c r="G41" t="s">
+        <v>147</v>
+      </c>
+      <c r="H41" t="s">
+        <v>147</v>
+      </c>
+      <c r="I41" s="1">
+        <v>44933</v>
+      </c>
+      <c r="J41" s="7">
+        <v>42.483620999999999</v>
+      </c>
+      <c r="K41" s="7">
+        <v>-71.185913999999997</v>
+      </c>
+      <c r="L41" s="6"/>
+      <c r="M41" t="s">
+        <v>54</v>
+      </c>
+      <c r="N41">
+        <v>1</v>
+      </c>
+      <c r="O41">
+        <v>44</v>
+      </c>
+      <c r="P41">
+        <v>8.4</v>
+      </c>
+      <c r="Q41">
+        <v>7.4</v>
+      </c>
+      <c r="R41">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>230</v>
+      </c>
+      <c r="C42" t="s">
+        <v>112</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="E42" t="s">
+        <v>178</v>
+      </c>
+      <c r="F42" t="s">
+        <v>163</v>
+      </c>
+      <c r="G42" t="s">
+        <v>147</v>
+      </c>
+      <c r="H42" t="s">
+        <v>147</v>
+      </c>
+      <c r="I42" s="1">
+        <v>44933</v>
+      </c>
+      <c r="J42" s="7">
+        <v>42.483620999999999</v>
+      </c>
+      <c r="K42" s="7">
+        <v>-71.185913999999997</v>
+      </c>
+      <c r="L42" s="6"/>
+      <c r="M42" t="s">
+        <v>54</v>
+      </c>
+      <c r="N42">
+        <v>1</v>
+      </c>
+      <c r="O42">
+        <v>46</v>
+      </c>
+      <c r="P42">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="Q42">
+        <v>7.3</v>
+      </c>
+      <c r="R42">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
playing with images and descriptions
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\Documents\DS_Projects\Analyducks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD09473-38ED-4DFA-A757-0F98A72E57C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67188434-93CC-4F5C-8170-B052D63EC376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EF9DEEC2-186D-4161-AB80-57C24753F6AE}"/>
   </bookViews>
@@ -1781,9 +1781,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B28BE0B7-C424-43DE-B13E-D21D7F7285C7}">
   <dimension ref="A1:V104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="88" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="88" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B99" sqref="B99"/>
+      <selection pane="topRight" activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
removed excess spacing, updated df
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\Documents\DS_Projects\Analyducks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A2310C2-555B-49BD-8822-E35DD8D07112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F714F4-7805-477C-A451-A49CAE80183C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="15750" xr2:uid="{EF9DEEC2-186D-4161-AB80-57C24753F6AE}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1036" uniqueCount="421">
   <si>
     <t>Duck</t>
   </si>
@@ -1296,19 +1296,37 @@
     <t>Goldwinger</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>e</t>
+    <t>Las Vegas</t>
+  </si>
+  <si>
+    <t>Las Vegas Cards</t>
+  </si>
+  <si>
+    <t>Flavortown</t>
+  </si>
+  <si>
+    <t>Koala</t>
+  </si>
+  <si>
+    <t>Clown</t>
+  </si>
+  <si>
+    <t>Elvis</t>
+  </si>
+  <si>
+    <t>Las Vegas Airport</t>
+  </si>
+  <si>
+    <t>NV</t>
+  </si>
+  <si>
+    <t>Nv</t>
+  </si>
+  <si>
+    <t>TN</t>
+  </si>
+  <si>
+    <t>Pigeon Forge</t>
   </si>
 </sst>
 </file>
@@ -1450,8 +1468,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{55715085-9AFB-4516-817F-DC3F49C2B133}" name="Table1" displayName="Table1" ref="A1:R104" totalsRowShown="0">
-  <autoFilter ref="A1:R104" xr:uid="{55715085-9AFB-4516-817F-DC3F49C2B133}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{55715085-9AFB-4516-817F-DC3F49C2B133}" name="Table1" displayName="Table1" ref="A1:R109" totalsRowShown="0">
+  <autoFilter ref="A1:R109" xr:uid="{55715085-9AFB-4516-817F-DC3F49C2B133}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R98">
     <sortCondition ref="I1:I98"/>
   </sortState>
@@ -1794,11 +1812,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B28BE0B7-C424-43DE-B13E-D21D7F7285C7}">
-  <dimension ref="A1:V104"/>
+  <dimension ref="A1:V109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="88" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="88" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B105" sqref="B105"/>
+      <selection pane="topRight" activeCell="Q103" sqref="Q103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1813,7 +1831,7 @@
     <col min="8" max="8" width="4.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="39.88671875" customWidth="1"/>
     <col min="13" max="13" width="7.109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.5546875" bestFit="1" customWidth="1"/>
@@ -7300,9 +7318,6 @@
       <c r="A100" t="s">
         <v>398</v>
       </c>
-      <c r="B100" t="s">
-        <v>410</v>
-      </c>
       <c r="C100" t="s">
         <v>112</v>
       </c>
@@ -7357,9 +7372,6 @@
       <c r="A101" t="s">
         <v>399</v>
       </c>
-      <c r="B101" t="s">
-        <v>411</v>
-      </c>
       <c r="C101" t="s">
         <v>112</v>
       </c>
@@ -7413,9 +7425,6 @@
       <c r="A102" t="s">
         <v>400</v>
       </c>
-      <c r="B102" t="s">
-        <v>412</v>
-      </c>
       <c r="C102" t="s">
         <v>112</v>
       </c>
@@ -7469,9 +7478,6 @@
       <c r="A103" t="s">
         <v>401</v>
       </c>
-      <c r="B103" t="s">
-        <v>413</v>
-      </c>
       <c r="C103" t="s">
         <v>112</v>
       </c>
@@ -7526,9 +7532,6 @@
       <c r="A104" t="s">
         <v>402</v>
       </c>
-      <c r="B104" t="s">
-        <v>414</v>
-      </c>
       <c r="C104" t="s">
         <v>112</v>
       </c>
@@ -7576,6 +7579,268 @@
       <c r="R104">
         <f>2+2/16</f>
         <v>2.125</v>
+      </c>
+    </row>
+    <row r="105" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>412</v>
+      </c>
+      <c r="C105" t="s">
+        <v>112</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="E105" t="s">
+        <v>420</v>
+      </c>
+      <c r="F105" t="s">
+        <v>419</v>
+      </c>
+      <c r="G105" t="s">
+        <v>147</v>
+      </c>
+      <c r="H105" t="s">
+        <v>147</v>
+      </c>
+      <c r="I105" s="1">
+        <v>45197</v>
+      </c>
+      <c r="J105" s="4">
+        <v>35.823491320947902</v>
+      </c>
+      <c r="K105" s="4">
+        <v>-83.562385482795094</v>
+      </c>
+      <c r="L105" s="6"/>
+      <c r="M105" t="s">
+        <v>50</v>
+      </c>
+      <c r="N105">
+        <v>1</v>
+      </c>
+      <c r="O105">
+        <v>20</v>
+      </c>
+      <c r="P105">
+        <f>2+5/16</f>
+        <v>2.3125</v>
+      </c>
+      <c r="Q105">
+        <f>1+11/16</f>
+        <v>1.6875</v>
+      </c>
+      <c r="R105">
+        <f>2+7/16</f>
+        <v>2.4375</v>
+      </c>
+    </row>
+    <row r="106" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>411</v>
+      </c>
+      <c r="C106" t="s">
+        <v>112</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="E106" t="s">
+        <v>410</v>
+      </c>
+      <c r="F106" t="s">
+        <v>417</v>
+      </c>
+      <c r="G106" t="s">
+        <v>147</v>
+      </c>
+      <c r="H106" t="s">
+        <v>147</v>
+      </c>
+      <c r="I106" s="1">
+        <v>45201</v>
+      </c>
+      <c r="J106" s="4">
+        <v>36.114481645923</v>
+      </c>
+      <c r="K106" s="4">
+        <v>-115.171873618758</v>
+      </c>
+      <c r="L106" s="6"/>
+      <c r="M106" t="s">
+        <v>50</v>
+      </c>
+      <c r="N106">
+        <v>1</v>
+      </c>
+      <c r="O106">
+        <v>70</v>
+      </c>
+      <c r="P106">
+        <f>2.625</f>
+        <v>2.625</v>
+      </c>
+      <c r="Q106">
+        <v>3</v>
+      </c>
+      <c r="R106">
+        <v>2.625</v>
+      </c>
+    </row>
+    <row r="107" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>414</v>
+      </c>
+      <c r="C107" t="s">
+        <v>112</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="E107" t="s">
+        <v>410</v>
+      </c>
+      <c r="F107" t="s">
+        <v>417</v>
+      </c>
+      <c r="G107" t="s">
+        <v>147</v>
+      </c>
+      <c r="H107" t="s">
+        <v>147</v>
+      </c>
+      <c r="I107" s="1">
+        <v>45201</v>
+      </c>
+      <c r="J107" s="4">
+        <v>36.114481645923</v>
+      </c>
+      <c r="K107" s="4">
+        <v>-115.171873618758</v>
+      </c>
+      <c r="L107" s="6"/>
+      <c r="M107" t="s">
+        <v>50</v>
+      </c>
+      <c r="N107">
+        <v>1</v>
+      </c>
+      <c r="O107">
+        <v>17</v>
+      </c>
+      <c r="P107">
+        <v>2.25</v>
+      </c>
+      <c r="Q107">
+        <f>1+14/16</f>
+        <v>1.875</v>
+      </c>
+      <c r="R107">
+        <f>1+14/16</f>
+        <v>1.875</v>
+      </c>
+    </row>
+    <row r="108" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>413</v>
+      </c>
+      <c r="C108" t="s">
+        <v>112</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="E108" t="s">
+        <v>410</v>
+      </c>
+      <c r="F108" t="s">
+        <v>417</v>
+      </c>
+      <c r="G108" t="s">
+        <v>147</v>
+      </c>
+      <c r="H108" t="s">
+        <v>147</v>
+      </c>
+      <c r="I108" s="1">
+        <v>45201</v>
+      </c>
+      <c r="J108" s="4">
+        <v>36.114481645923</v>
+      </c>
+      <c r="K108" s="4">
+        <v>-115.171873618758</v>
+      </c>
+      <c r="L108" s="6"/>
+      <c r="M108" t="s">
+        <v>50</v>
+      </c>
+      <c r="N108">
+        <v>1</v>
+      </c>
+      <c r="O108">
+        <v>15</v>
+      </c>
+      <c r="P108">
+        <v>2</v>
+      </c>
+      <c r="Q108">
+        <f>1+13/16</f>
+        <v>1.8125</v>
+      </c>
+      <c r="R108">
+        <v>1.875</v>
+      </c>
+    </row>
+    <row r="109" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>415</v>
+      </c>
+      <c r="C109" t="s">
+        <v>112</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="E109" t="s">
+        <v>410</v>
+      </c>
+      <c r="F109" t="s">
+        <v>418</v>
+      </c>
+      <c r="G109" t="s">
+        <v>147</v>
+      </c>
+      <c r="H109" t="s">
+        <v>147</v>
+      </c>
+      <c r="I109" s="1">
+        <v>45204</v>
+      </c>
+      <c r="J109" s="4">
+        <v>36.083568911204402</v>
+      </c>
+      <c r="K109" s="4">
+        <v>-115.149256886367</v>
+      </c>
+      <c r="L109" s="6"/>
+      <c r="M109" t="s">
+        <v>50</v>
+      </c>
+      <c r="N109">
+        <v>1</v>
+      </c>
+      <c r="O109">
+        <v>54</v>
+      </c>
+      <c r="P109">
+        <v>3</v>
+      </c>
+      <c r="Q109">
+        <v>2.625</v>
+      </c>
+      <c r="R109">
+        <v>3.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated title, got background diff color
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\Documents\DS_Projects\Analyducks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F714F4-7805-477C-A451-A49CAE80183C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E244E940-671E-48FB-BF73-6AD90115715D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="15750" xr2:uid="{EF9DEEC2-186D-4161-AB80-57C24753F6AE}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{EF9DEEC2-186D-4161-AB80-57C24753F6AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Ducks" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1036" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1036" uniqueCount="422">
   <si>
     <t>Duck</t>
   </si>
@@ -1327,6 +1327,9 @@
   </si>
   <si>
     <t>Pigeon Forge</t>
+  </si>
+  <si>
+    <t>Katie</t>
   </si>
 </sst>
 </file>
@@ -1815,8 +1818,8 @@
   <dimension ref="A1:V109"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A84" zoomScale="88" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q103" sqref="Q103"/>
+      <pane xSplit="2" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M106" sqref="M106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7614,7 +7617,7 @@
       </c>
       <c r="L105" s="6"/>
       <c r="M105" t="s">
-        <v>50</v>
+        <v>421</v>
       </c>
       <c r="N105">
         <v>1</v>

</xml_diff>

<commit_message>
updating analyducks page for portfolio
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\Documents\DS_Projects\Analyducks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E244E940-671E-48FB-BF73-6AD90115715D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D5739E-C74E-4E79-A8C9-252FC3BFA42A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{EF9DEEC2-186D-4161-AB80-57C24753F6AE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EF9DEEC2-186D-4161-AB80-57C24753F6AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Ducks" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1036" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="422">
   <si>
     <t>Duck</t>
   </si>
@@ -1320,9 +1320,6 @@
     <t>NV</t>
   </si>
   <si>
-    <t>Nv</t>
-  </si>
-  <si>
     <t>TN</t>
   </si>
   <si>
@@ -1330,6 +1327,9 @@
   </si>
   <si>
     <t>Katie</t>
+  </si>
+  <si>
+    <t>QQ</t>
   </si>
 </sst>
 </file>
@@ -1817,9 +1817,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B28BE0B7-C424-43DE-B13E-D21D7F7285C7}">
   <dimension ref="A1:V109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="88" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M106" sqref="M106"/>
+    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="88" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F109" sqref="F109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2593,6 +2593,9 @@
       <c r="E14" t="s">
         <v>152</v>
       </c>
+      <c r="F14" t="s">
+        <v>421</v>
+      </c>
       <c r="G14" t="s">
         <v>60</v>
       </c>
@@ -2647,6 +2650,9 @@
       <c r="E15" t="s">
         <v>167</v>
       </c>
+      <c r="F15" t="s">
+        <v>421</v>
+      </c>
       <c r="G15" t="s">
         <v>150</v>
       </c>
@@ -3097,6 +3103,9 @@
       <c r="E23" t="s">
         <v>149</v>
       </c>
+      <c r="F23" t="s">
+        <v>421</v>
+      </c>
       <c r="G23" t="s">
         <v>42</v>
       </c>
@@ -3151,6 +3160,9 @@
       <c r="E24" t="s">
         <v>149</v>
       </c>
+      <c r="F24" t="s">
+        <v>421</v>
+      </c>
       <c r="G24" t="s">
         <v>42</v>
       </c>
@@ -3205,6 +3217,9 @@
       <c r="E25" t="s">
         <v>149</v>
       </c>
+      <c r="F25" t="s">
+        <v>421</v>
+      </c>
       <c r="G25" t="s">
         <v>42</v>
       </c>
@@ -3258,6 +3273,9 @@
       <c r="E26" t="s">
         <v>153</v>
       </c>
+      <c r="F26" t="s">
+        <v>421</v>
+      </c>
       <c r="G26" t="s">
         <v>42</v>
       </c>
@@ -3312,6 +3330,9 @@
       <c r="E27" t="s">
         <v>149</v>
       </c>
+      <c r="F27" t="s">
+        <v>421</v>
+      </c>
       <c r="G27" t="s">
         <v>42</v>
       </c>
@@ -3422,6 +3443,9 @@
       <c r="E29" t="s">
         <v>41</v>
       </c>
+      <c r="F29" t="s">
+        <v>421</v>
+      </c>
       <c r="G29" t="s">
         <v>148</v>
       </c>
@@ -4117,7 +4141,9 @@
       <c r="K41" s="4">
         <v>-71.185913999999997</v>
       </c>
-      <c r="L41" s="6"/>
+      <c r="L41" s="6">
+        <v>1</v>
+      </c>
       <c r="M41" t="s">
         <v>54</v>
       </c>
@@ -4283,7 +4309,9 @@
       <c r="K44" s="4">
         <v>-73.151848000000001</v>
       </c>
-      <c r="L44" s="6"/>
+      <c r="L44" s="6">
+        <v>2</v>
+      </c>
       <c r="M44" t="s">
         <v>54</v>
       </c>
@@ -4449,7 +4477,9 @@
       <c r="K47" s="4">
         <v>-72.386257999999998</v>
       </c>
-      <c r="L47" s="6"/>
+      <c r="L47" s="6">
+        <v>3</v>
+      </c>
       <c r="M47" t="s">
         <v>50</v>
       </c>
@@ -4473,6 +4503,9 @@
       <c r="A48" t="s">
         <v>245</v>
       </c>
+      <c r="B48">
+        <v>21</v>
+      </c>
       <c r="C48" t="s">
         <v>112</v>
       </c>
@@ -4500,7 +4533,9 @@
       <c r="K48" s="4">
         <v>-72.386257999999998</v>
       </c>
-      <c r="L48" s="6"/>
+      <c r="L48" s="6">
+        <v>4</v>
+      </c>
       <c r="M48" t="s">
         <v>50</v>
       </c>
@@ -4554,7 +4589,9 @@
       <c r="K49" s="4">
         <v>-72.386257999999998</v>
       </c>
-      <c r="L49" s="6"/>
+      <c r="L49" s="6">
+        <v>5</v>
+      </c>
       <c r="M49" t="s">
         <v>54</v>
       </c>
@@ -4667,7 +4704,9 @@
       <c r="K51" s="4">
         <v>-72.386257999999998</v>
       </c>
-      <c r="L51" s="6"/>
+      <c r="L51" s="6">
+        <v>6</v>
+      </c>
       <c r="M51" t="s">
         <v>54</v>
       </c>
@@ -4750,6 +4789,9 @@
       <c r="A53" t="s">
         <v>246</v>
       </c>
+      <c r="B53">
+        <v>22</v>
+      </c>
       <c r="C53" t="s">
         <v>112</v>
       </c>
@@ -4777,7 +4819,9 @@
       <c r="K53" s="4">
         <v>-71.034631000000005</v>
       </c>
-      <c r="L53" s="6"/>
+      <c r="L53" s="6">
+        <v>7</v>
+      </c>
       <c r="M53" t="s">
         <v>50</v>
       </c>
@@ -4831,7 +4875,9 @@
       <c r="K54" s="4">
         <v>-71.034631000000005</v>
       </c>
-      <c r="L54" s="6"/>
+      <c r="L54" s="6">
+        <v>8</v>
+      </c>
       <c r="M54" t="s">
         <v>50</v>
       </c>
@@ -5079,6 +5125,9 @@
       <c r="A59" t="s">
         <v>260</v>
       </c>
+      <c r="B59">
+        <v>1</v>
+      </c>
       <c r="C59" t="s">
         <v>132</v>
       </c>
@@ -5132,6 +5181,9 @@
       <c r="A60" t="s">
         <v>276</v>
       </c>
+      <c r="B60">
+        <v>2</v>
+      </c>
       <c r="C60" t="s">
         <v>112</v>
       </c>
@@ -5330,7 +5382,9 @@
       <c r="K63" s="4">
         <v>-71.079604205770494</v>
       </c>
-      <c r="L63" s="6"/>
+      <c r="L63" s="6">
+        <v>9</v>
+      </c>
       <c r="M63" t="s">
         <v>50</v>
       </c>
@@ -5386,7 +5440,9 @@
       <c r="K64" s="4">
         <v>-71.046275530971798</v>
       </c>
-      <c r="L64" s="6"/>
+      <c r="L64" s="6">
+        <v>10</v>
+      </c>
       <c r="M64" t="s">
         <v>50</v>
       </c>
@@ -5441,7 +5497,9 @@
       <c r="K65" s="4">
         <v>-71.046275530971798</v>
       </c>
-      <c r="L65" s="6"/>
+      <c r="L65" s="6">
+        <v>11</v>
+      </c>
       <c r="M65" t="s">
         <v>50</v>
       </c>
@@ -5467,6 +5525,9 @@
       <c r="A66" t="s">
         <v>291</v>
       </c>
+      <c r="B66">
+        <v>3</v>
+      </c>
       <c r="C66" t="s">
         <v>112</v>
       </c>
@@ -5521,6 +5582,9 @@
       <c r="A67" t="s">
         <v>292</v>
       </c>
+      <c r="B67">
+        <v>4</v>
+      </c>
       <c r="C67" t="s">
         <v>112</v>
       </c>
@@ -5662,7 +5726,9 @@
       <c r="K69" s="4">
         <v>-71.185913999999997</v>
       </c>
-      <c r="L69" s="6"/>
+      <c r="L69" s="6">
+        <v>12</v>
+      </c>
       <c r="M69" t="s">
         <v>50</v>
       </c>
@@ -5717,7 +5783,9 @@
       <c r="K70" s="4">
         <v>-71.185913999999997</v>
       </c>
-      <c r="L70" s="6"/>
+      <c r="L70" s="6">
+        <v>13</v>
+      </c>
       <c r="M70" t="s">
         <v>50</v>
       </c>
@@ -5812,6 +5880,9 @@
       <c r="E72" t="s">
         <v>297</v>
       </c>
+      <c r="F72" t="s">
+        <v>421</v>
+      </c>
       <c r="G72" t="s">
         <v>294</v>
       </c>
@@ -5827,7 +5898,9 @@
       <c r="K72" s="4">
         <v>10.8694581371567</v>
       </c>
-      <c r="L72" s="6"/>
+      <c r="L72" s="6">
+        <v>14</v>
+      </c>
       <c r="M72" t="s">
         <v>50</v>
       </c>
@@ -5863,6 +5936,9 @@
       <c r="E73" t="s">
         <v>288</v>
       </c>
+      <c r="F73" t="s">
+        <v>421</v>
+      </c>
       <c r="G73" t="s">
         <v>294</v>
       </c>
@@ -5878,7 +5954,9 @@
       <c r="K73" s="4">
         <v>12.3372370361033</v>
       </c>
-      <c r="L73" s="6"/>
+      <c r="L73" s="6">
+        <v>15</v>
+      </c>
       <c r="M73" t="s">
         <v>50</v>
       </c>
@@ -5915,6 +5993,9 @@
       <c r="E74" t="s">
         <v>288</v>
       </c>
+      <c r="F74" t="s">
+        <v>421</v>
+      </c>
       <c r="G74" t="s">
         <v>294</v>
       </c>
@@ -5930,7 +6011,9 @@
       <c r="K74" s="4">
         <v>12.3372370361033</v>
       </c>
-      <c r="L74" s="6"/>
+      <c r="L74" s="6">
+        <v>16</v>
+      </c>
       <c r="M74" t="s">
         <v>50</v>
       </c>
@@ -5967,6 +6050,9 @@
       <c r="E75" t="s">
         <v>288</v>
       </c>
+      <c r="F75" t="s">
+        <v>421</v>
+      </c>
       <c r="G75" t="s">
         <v>294</v>
       </c>
@@ -5982,7 +6068,9 @@
       <c r="K75" s="4">
         <v>12.3372370361033</v>
       </c>
-      <c r="L75" s="6"/>
+      <c r="L75" s="6">
+        <v>17</v>
+      </c>
       <c r="M75" t="s">
         <v>50</v>
       </c>
@@ -6019,6 +6107,9 @@
       <c r="E76" t="s">
         <v>288</v>
       </c>
+      <c r="F76" t="s">
+        <v>421</v>
+      </c>
       <c r="G76" t="s">
         <v>294</v>
       </c>
@@ -6034,7 +6125,9 @@
       <c r="K76" s="4">
         <v>12.3372370361033</v>
       </c>
-      <c r="L76" s="6"/>
+      <c r="L76" s="6">
+        <v>18</v>
+      </c>
       <c r="M76" t="s">
         <v>50</v>
       </c>
@@ -6072,6 +6165,9 @@
       <c r="E77" t="s">
         <v>284</v>
       </c>
+      <c r="F77" t="s">
+        <v>421</v>
+      </c>
       <c r="G77" t="s">
         <v>294</v>
       </c>
@@ -6087,7 +6183,9 @@
       <c r="K77" s="4">
         <v>12.5198672082531</v>
       </c>
-      <c r="L77" s="6"/>
+      <c r="L77" s="6">
+        <v>19</v>
+      </c>
       <c r="M77" t="s">
         <v>50</v>
       </c>
@@ -6124,6 +6222,9 @@
       <c r="E78" t="s">
         <v>284</v>
       </c>
+      <c r="F78" t="s">
+        <v>421</v>
+      </c>
       <c r="G78" t="s">
         <v>294</v>
       </c>
@@ -6139,7 +6240,9 @@
       <c r="K78" s="4">
         <v>12.5198672082531</v>
       </c>
-      <c r="L78" s="6"/>
+      <c r="L78" s="6">
+        <v>20</v>
+      </c>
       <c r="M78" t="s">
         <v>50</v>
       </c>
@@ -6175,6 +6278,9 @@
       <c r="E79" t="s">
         <v>284</v>
       </c>
+      <c r="F79" t="s">
+        <v>421</v>
+      </c>
       <c r="G79" t="s">
         <v>294</v>
       </c>
@@ -6190,7 +6296,9 @@
       <c r="K79" s="4">
         <v>12.5198672082531</v>
       </c>
-      <c r="L79" s="6"/>
+      <c r="L79" s="6">
+        <v>21</v>
+      </c>
       <c r="M79" t="s">
         <v>50</v>
       </c>
@@ -6217,6 +6325,9 @@
       <c r="A80" t="s">
         <v>307</v>
       </c>
+      <c r="B80">
+        <v>5</v>
+      </c>
       <c r="C80" t="s">
         <v>112</v>
       </c>
@@ -6244,7 +6355,9 @@
       <c r="K80" s="4">
         <v>-69.957497000000004</v>
       </c>
-      <c r="L80" s="6"/>
+      <c r="L80" s="6">
+        <v>22</v>
+      </c>
       <c r="M80" t="s">
         <v>50</v>
       </c>
@@ -6301,7 +6414,9 @@
       <c r="K81" s="4">
         <v>-69.957497000000004</v>
       </c>
-      <c r="L81" s="6"/>
+      <c r="L81" s="6">
+        <v>23</v>
+      </c>
       <c r="M81" t="s">
         <v>50</v>
       </c>
@@ -6327,6 +6442,9 @@
       <c r="A82" t="s">
         <v>311</v>
       </c>
+      <c r="B82">
+        <v>6</v>
+      </c>
       <c r="C82" t="s">
         <v>112</v>
       </c>
@@ -6354,7 +6472,9 @@
       <c r="K82" s="4">
         <v>-69.957497000000004</v>
       </c>
-      <c r="L82" s="6"/>
+      <c r="L82" s="6">
+        <v>24</v>
+      </c>
       <c r="M82" t="s">
         <v>50</v>
       </c>
@@ -6380,6 +6500,9 @@
       <c r="A83" t="s">
         <v>312</v>
       </c>
+      <c r="B83">
+        <v>7</v>
+      </c>
       <c r="C83" t="s">
         <v>112</v>
       </c>
@@ -6407,7 +6530,9 @@
       <c r="K83" s="4">
         <v>-69.957497000000004</v>
       </c>
-      <c r="L83" s="6"/>
+      <c r="L83" s="6">
+        <v>25</v>
+      </c>
       <c r="M83" t="s">
         <v>50</v>
       </c>
@@ -6464,7 +6589,9 @@
       <c r="K84" s="4">
         <v>-97.667443945545301</v>
       </c>
-      <c r="L84" s="6"/>
+      <c r="L84" s="6">
+        <v>26</v>
+      </c>
       <c r="M84" t="s">
         <v>50</v>
       </c>
@@ -6520,7 +6647,9 @@
       <c r="K85" s="4">
         <v>-97.667443945545301</v>
       </c>
-      <c r="L85" s="6"/>
+      <c r="L85" s="6">
+        <v>27</v>
+      </c>
       <c r="M85" t="s">
         <v>50</v>
       </c>
@@ -6545,6 +6674,9 @@
       <c r="A86" t="s">
         <v>318</v>
       </c>
+      <c r="B86">
+        <v>8</v>
+      </c>
       <c r="C86" t="s">
         <v>112</v>
       </c>
@@ -6572,7 +6704,9 @@
       <c r="K86" s="4">
         <v>-79.932914999999994</v>
       </c>
-      <c r="L86" s="6"/>
+      <c r="L86" s="6">
+        <v>28</v>
+      </c>
       <c r="M86" t="s">
         <v>50</v>
       </c>
@@ -6596,6 +6730,9 @@
       <c r="A87" t="s">
         <v>319</v>
       </c>
+      <c r="B87">
+        <v>9</v>
+      </c>
       <c r="C87" t="s">
         <v>112</v>
       </c>
@@ -6739,7 +6876,9 @@
       <c r="K89" s="4">
         <v>-77.130231786099699</v>
       </c>
-      <c r="L89" s="6"/>
+      <c r="L89" s="6">
+        <v>29</v>
+      </c>
       <c r="M89" t="s">
         <v>50</v>
       </c>
@@ -6852,7 +6991,9 @@
       <c r="K91" s="4">
         <v>-77.188013773757405</v>
       </c>
-      <c r="L91" s="6"/>
+      <c r="L91" s="6">
+        <v>30</v>
+      </c>
       <c r="M91" t="s">
         <v>50</v>
       </c>
@@ -6908,7 +7049,9 @@
       <c r="K92" s="4">
         <v>-77.188013773757405</v>
       </c>
-      <c r="L92" s="6"/>
+      <c r="L92" s="6">
+        <v>31</v>
+      </c>
       <c r="M92" t="s">
         <v>54</v>
       </c>
@@ -6964,7 +7107,9 @@
       <c r="K93" s="4">
         <v>-77.188013773757405</v>
       </c>
-      <c r="L93" s="6"/>
+      <c r="L93" s="6">
+        <v>32</v>
+      </c>
       <c r="M93" t="s">
         <v>50</v>
       </c>
@@ -7019,7 +7164,9 @@
       <c r="K94" s="4">
         <v>-93.166926000000004</v>
       </c>
-      <c r="L94" s="6"/>
+      <c r="L94" s="6">
+        <v>33</v>
+      </c>
       <c r="M94" t="s">
         <v>50</v>
       </c>
@@ -7160,6 +7307,9 @@
       <c r="A97" t="s">
         <v>348</v>
       </c>
+      <c r="B97">
+        <v>20</v>
+      </c>
       <c r="C97" t="s">
         <v>112</v>
       </c>
@@ -7187,7 +7337,9 @@
       <c r="K97" s="4">
         <v>-77.114897400000004</v>
       </c>
-      <c r="L97" s="6"/>
+      <c r="L97" s="6">
+        <v>34</v>
+      </c>
       <c r="M97" t="s">
         <v>50</v>
       </c>
@@ -7242,7 +7394,9 @@
       <c r="K98" s="4">
         <v>-77.114897400000004</v>
       </c>
-      <c r="L98" s="6"/>
+      <c r="L98" s="6">
+        <v>35</v>
+      </c>
       <c r="M98" t="s">
         <v>50</v>
       </c>
@@ -7297,7 +7451,9 @@
       <c r="K99" s="4">
         <v>-80.871899999999997</v>
       </c>
-      <c r="L99" s="6"/>
+      <c r="L99" s="6">
+        <v>36</v>
+      </c>
       <c r="M99" t="s">
         <v>50</v>
       </c>
@@ -7321,6 +7477,9 @@
       <c r="A100" t="s">
         <v>398</v>
       </c>
+      <c r="B100">
+        <v>10</v>
+      </c>
       <c r="C100" t="s">
         <v>112</v>
       </c>
@@ -7348,7 +7507,9 @@
       <c r="K100" s="4">
         <v>-80.861380999999994</v>
       </c>
-      <c r="L100" s="6"/>
+      <c r="L100" s="6">
+        <v>37</v>
+      </c>
       <c r="M100" t="s">
         <v>50</v>
       </c>
@@ -7375,6 +7536,9 @@
       <c r="A101" t="s">
         <v>399</v>
       </c>
+      <c r="B101">
+        <v>11</v>
+      </c>
       <c r="C101" t="s">
         <v>112</v>
       </c>
@@ -7402,7 +7566,9 @@
       <c r="K101" s="4">
         <v>-80.861380999999994</v>
       </c>
-      <c r="L101" s="6"/>
+      <c r="L101" s="6">
+        <v>38</v>
+      </c>
       <c r="M101" t="s">
         <v>50</v>
       </c>
@@ -7428,6 +7594,9 @@
       <c r="A102" t="s">
         <v>400</v>
       </c>
+      <c r="B102">
+        <v>12</v>
+      </c>
       <c r="C102" t="s">
         <v>112</v>
       </c>
@@ -7455,7 +7624,9 @@
       <c r="K102" s="4">
         <v>-80.861380999999994</v>
       </c>
-      <c r="L102" s="6"/>
+      <c r="L102" s="6">
+        <v>39</v>
+      </c>
       <c r="M102" t="s">
         <v>50</v>
       </c>
@@ -7481,6 +7652,9 @@
       <c r="A103" t="s">
         <v>401</v>
       </c>
+      <c r="B103">
+        <v>13</v>
+      </c>
       <c r="C103" t="s">
         <v>112</v>
       </c>
@@ -7508,7 +7682,9 @@
       <c r="K103" s="4">
         <v>-80.861380999999994</v>
       </c>
-      <c r="L103" s="6"/>
+      <c r="L103" s="6">
+        <v>40</v>
+      </c>
       <c r="M103" t="s">
         <v>50</v>
       </c>
@@ -7535,6 +7711,9 @@
       <c r="A104" t="s">
         <v>402</v>
       </c>
+      <c r="B104">
+        <v>14</v>
+      </c>
       <c r="C104" t="s">
         <v>112</v>
       </c>
@@ -7562,7 +7741,9 @@
       <c r="K104" s="4">
         <v>-72.381726</v>
       </c>
-      <c r="L104" s="6"/>
+      <c r="L104" s="6">
+        <v>41</v>
+      </c>
       <c r="M104" t="s">
         <v>407</v>
       </c>
@@ -7588,6 +7769,9 @@
       <c r="A105" t="s">
         <v>412</v>
       </c>
+      <c r="B105">
+        <v>15</v>
+      </c>
       <c r="C105" t="s">
         <v>112</v>
       </c>
@@ -7595,10 +7779,10 @@
         <v>412</v>
       </c>
       <c r="E105" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F105" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G105" t="s">
         <v>147</v>
@@ -7615,9 +7799,11 @@
       <c r="K105" s="4">
         <v>-83.562385482795094</v>
       </c>
-      <c r="L105" s="6"/>
+      <c r="L105" s="6">
+        <v>42</v>
+      </c>
       <c r="M105" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="N105">
         <v>1</v>
@@ -7642,6 +7828,9 @@
       <c r="A106" t="s">
         <v>411</v>
       </c>
+      <c r="B106">
+        <v>16</v>
+      </c>
       <c r="C106" t="s">
         <v>112</v>
       </c>
@@ -7669,7 +7858,9 @@
       <c r="K106" s="4">
         <v>-115.171873618758</v>
       </c>
-      <c r="L106" s="6"/>
+      <c r="L106" s="6">
+        <v>43</v>
+      </c>
       <c r="M106" t="s">
         <v>50</v>
       </c>
@@ -7694,6 +7885,9 @@
       <c r="A107" t="s">
         <v>414</v>
       </c>
+      <c r="B107">
+        <v>17</v>
+      </c>
       <c r="C107" t="s">
         <v>112</v>
       </c>
@@ -7721,7 +7915,9 @@
       <c r="K107" s="4">
         <v>-115.171873618758</v>
       </c>
-      <c r="L107" s="6"/>
+      <c r="L107" s="6">
+        <v>44</v>
+      </c>
       <c r="M107" t="s">
         <v>50</v>
       </c>
@@ -7747,6 +7943,9 @@
       <c r="A108" t="s">
         <v>413</v>
       </c>
+      <c r="B108">
+        <v>18</v>
+      </c>
       <c r="C108" t="s">
         <v>112</v>
       </c>
@@ -7774,7 +7973,9 @@
       <c r="K108" s="4">
         <v>-115.171873618758</v>
       </c>
-      <c r="L108" s="6"/>
+      <c r="L108" s="6">
+        <v>45</v>
+      </c>
       <c r="M108" t="s">
         <v>50</v>
       </c>
@@ -7799,6 +8000,9 @@
       <c r="A109" t="s">
         <v>415</v>
       </c>
+      <c r="B109">
+        <v>19</v>
+      </c>
       <c r="C109" t="s">
         <v>112</v>
       </c>
@@ -7809,7 +8013,7 @@
         <v>410</v>
       </c>
       <c r="F109" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="G109" t="s">
         <v>147</v>
@@ -7826,7 +8030,9 @@
       <c r="K109" s="4">
         <v>-115.149256886367</v>
       </c>
-      <c r="L109" s="6"/>
+      <c r="L109" s="6">
+        <v>46</v>
+      </c>
       <c r="M109" t="s">
         <v>50</v>
       </c>

</xml_diff>